<commit_message>
Adding 4 new regions to the model
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-DK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F39D87-D6B9-40D1-9326-C41307F19AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{46F39D87-D6B9-40D1-9326-C41307F19AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{746BD033-5960-43A8-BD8C-D1F20A120AE8}"/>
   <bookViews>
-    <workbookView xWindow="16188" yWindow="0" windowWidth="21960" windowHeight="15468" tabRatio="853" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3218" yWindow="3218" windowWidth="16875" windowHeight="10522" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="22" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="159">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -667,6 +667,18 @@
   </si>
   <si>
     <t xml:space="preserve">Source: DK2025 </t>
+  </si>
+  <si>
+    <t>DKISLBH</t>
+  </si>
+  <si>
+    <t>DKISL1</t>
+  </si>
+  <si>
+    <t>DKISL2</t>
+  </si>
+  <si>
+    <t>DKISL3</t>
   </si>
 </sst>
 </file>
@@ -871,6 +883,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1155,7 +1168,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="5"/>
@@ -1185,12 +1198,11 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="4" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1305,41 +1317,41 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="17" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="16" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="16" applyBorder="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="17" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="17" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="17" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="16" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="16" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="16" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="16" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="17" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="16" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="18">
     <cellStyle name="5x indented GHG Textfiels" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="AggOrange_CRFReport-template" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="AggOrange9_CRFReport-template" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="CustomizationCells" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Euro" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8"/>
     <cellStyle name="InputCells" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="17" builtinId="8"/>
     <cellStyle name="Normal 10" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 4" xfId="17" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 4" xfId="16" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal GHG Numbers (0.00)" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Normal GHG Textfiels Bold" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal GHG-Shade" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Normale_B2020" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Percent" xfId="14" builtinId="5"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Обычный_CRF2002 (1)" xfId="16" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Prozent" xfId="14" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный_CRF2002 (1)" xfId="15" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1553,7 +1565,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1882,16 +1894,16 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.53125" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" customWidth="1"/>
     <col min="5" max="5" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
@@ -1908,7 +1920,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="51">
         <v>42843</v>
       </c>
@@ -1926,7 +1938,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="51">
         <v>42702</v>
       </c>
@@ -1944,7 +1956,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="51">
         <v>42604</v>
       </c>
@@ -1962,7 +1974,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="51">
         <v>42549</v>
       </c>
@@ -1980,7 +1992,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="51">
         <v>42115</v>
       </c>
@@ -1997,7 +2009,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="51">
         <v>42341</v>
       </c>
@@ -2015,7 +2027,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="51">
         <v>42311</v>
       </c>
@@ -2033,7 +2045,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="51">
         <v>42264</v>
       </c>
@@ -2051,7 +2063,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="51">
         <v>42264</v>
       </c>
@@ -2069,7 +2081,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="51">
         <v>42264</v>
       </c>
@@ -2087,7 +2099,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="51">
         <v>42264</v>
       </c>
@@ -2105,7 +2117,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="51">
         <v>42264</v>
       </c>
@@ -2136,19 +2148,21 @@
   </sheetPr>
   <dimension ref="A3:S39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1328125" customWidth="1"/>
+    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" customWidth="1"/>
+    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
       <c r="B3" s="12" t="s">
         <v>10</v>
@@ -2159,7 +2173,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="13" t="s">
         <v>16</v>
@@ -2177,7 +2191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>57</v>
       </c>
@@ -2216,7 +2230,7 @@
       </c>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C6" s="3" t="s">
         <v>78</v>
       </c>
@@ -2252,10 +2266,12 @@
       </c>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="76" t="s">
+        <v>155</v>
+      </c>
       <c r="E7" s="19" t="s">
         <v>68</v>
       </c>
@@ -2278,10 +2294,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="76" t="s">
+        <v>156</v>
+      </c>
       <c r="E8" s="19" t="s">
         <v>69</v>
       </c>
@@ -2305,23 +2323,27 @@
       </c>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="76" t="s">
+        <v>157</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C10" s="76" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2339,7 +2361,7 @@
       <c r="Q12" s="21"/>
       <c r="R12" s="21"/>
     </row>
-    <row r="13" spans="1:19" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2355,7 +2377,7 @@
       <c r="Q13" s="21"/>
       <c r="R13" s="21"/>
     </row>
-    <row r="14" spans="1:19" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2365,7 +2387,7 @@
       <c r="Q14" s="21"/>
       <c r="R14" s="21"/>
     </row>
-    <row r="15" spans="1:19" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2375,7 +2397,7 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="21"/>
     </row>
-    <row r="16" spans="1:19" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2385,7 +2407,7 @@
       <c r="Q16" s="21"/>
       <c r="R16" s="21"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2395,7 +2417,7 @@
       <c r="Q17" s="21"/>
       <c r="R17" s="21"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2405,69 +2427,69 @@
       <c r="Q18" s="21"/>
       <c r="R18" s="21"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
     </row>
   </sheetData>
@@ -2487,40 +2509,40 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="70" t="s">
         <v>128</v>
       </c>
@@ -2534,7 +2556,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="18">
         <v>1</v>
       </c>
@@ -2548,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="18">
         <v>1</v>
       </c>
@@ -2562,7 +2584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="18">
         <v>1</v>
       </c>
@@ -2576,7 +2598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="18">
         <v>1</v>
       </c>
@@ -2590,7 +2612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="18">
         <v>1</v>
       </c>
@@ -2604,7 +2626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="18">
         <v>1</v>
       </c>
@@ -2618,7 +2640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="18">
         <v>1</v>
       </c>
@@ -2632,7 +2654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="18">
         <v>1</v>
       </c>
@@ -2646,7 +2668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="18">
         <v>1</v>
       </c>
@@ -2660,7 +2682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="18">
         <v>1</v>
       </c>
@@ -2674,7 +2696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="18">
         <v>1</v>
       </c>
@@ -2688,7 +2710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="18">
         <v>1</v>
       </c>
@@ -2702,7 +2724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="18">
         <v>1</v>
       </c>
@@ -2716,7 +2738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="18">
         <v>1</v>
       </c>
@@ -2730,7 +2752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="18">
         <v>1</v>
       </c>
@@ -2744,7 +2766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="18">
         <v>1</v>
       </c>
@@ -2758,7 +2780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="18">
         <v>1</v>
       </c>
@@ -2772,7 +2794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="18">
         <v>1</v>
       </c>
@@ -2784,7 +2806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="18">
         <v>1</v>
       </c>
@@ -2796,7 +2818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="18">
         <v>1</v>
       </c>
@@ -2808,7 +2830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="18">
         <v>1</v>
       </c>
@@ -2818,7 +2840,7 @@
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="18">
         <v>1</v>
       </c>
@@ -2828,7 +2850,7 @@
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="18">
         <v>1</v>
       </c>
@@ -2838,7 +2860,7 @@
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="18">
         <v>1</v>
       </c>
@@ -2848,7 +2870,7 @@
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="18">
         <v>1</v>
       </c>
@@ -2858,7 +2880,7 @@
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="18">
         <v>1</v>
       </c>
@@ -2868,7 +2890,7 @@
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="18">
         <v>1</v>
       </c>
@@ -2878,7 +2900,7 @@
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="18">
         <v>1</v>
       </c>
@@ -2888,7 +2910,7 @@
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="18">
         <v>1</v>
       </c>
@@ -2898,7 +2920,7 @@
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="18">
         <v>1</v>
       </c>
@@ -2908,7 +2930,7 @@
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" s="18">
         <v>1</v>
       </c>
@@ -2916,7 +2938,7 @@
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" s="18">
         <v>1</v>
       </c>
@@ -2924,7 +2946,7 @@
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B45" s="18">
         <v>1</v>
       </c>
@@ -2932,7 +2954,7 @@
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B46" s="18">
         <v>1</v>
       </c>
@@ -2940,7 +2962,7 @@
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B47" s="18">
         <v>1</v>
       </c>
@@ -2948,7 +2970,7 @@
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B48" s="18">
         <v>1</v>
       </c>
@@ -2956,7 +2978,7 @@
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" s="18">
         <v>1</v>
       </c>
@@ -2964,7 +2986,7 @@
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" s="18">
         <v>1</v>
       </c>
@@ -2972,7 +2994,7 @@
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" s="18">
         <v>1</v>
       </c>
@@ -2980,7 +3002,7 @@
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" s="18">
         <v>1</v>
       </c>
@@ -2988,7 +3010,7 @@
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" s="18">
         <v>1</v>
       </c>
@@ -3012,20 +3034,20 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="1" max="1" width="2.86328125" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.86328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.46484375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
         <v>45</v>
       </c>
@@ -3039,19 +3061,19 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="5" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
@@ -3100,7 +3122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
@@ -3143,7 +3165,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>86</v>
       </c>
@@ -3159,60 +3181,60 @@
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="E10" s="7"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="E11" s="7"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="E12" s="7"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="E13" s="7"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="E14" s="7"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="E15" s="7"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="19" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" ht="15" x14ac:dyDescent="0.4">
       <c r="B19" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:16" ht="17.25" x14ac:dyDescent="0.45">
       <c r="B21" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="13" t="s">
         <v>20</v>
       </c>
@@ -3259,7 +3281,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
         <v>4</v>
       </c>
@@ -3276,7 +3298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D25" t="s">
         <v>4</v>
       </c>
@@ -3309,18 +3331,18 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="1" max="1" width="2.46484375" customWidth="1"/>
     <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B3" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B4" s="27" t="s">
         <v>34</v>
       </c>
@@ -3328,7 +3350,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="24" t="s">
         <v>36</v>
       </c>
@@ -3336,7 +3358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>37</v>
       </c>
@@ -3344,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" s="25" t="s">
         <v>38</v>
       </c>
@@ -3352,7 +3374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" s="25" t="s">
         <v>39</v>
       </c>
@@ -3360,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="25" t="s">
         <v>80</v>
       </c>
@@ -3383,32 +3405,32 @@
   </sheetPr>
   <dimension ref="B3:CM58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F28" sqref="F25:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="8"/>
+    <col min="1" max="1" width="9.1328125" style="8"/>
     <col min="2" max="2" width="13.6640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.46484375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.44140625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="8"/>
+    <col min="7" max="7" width="6.46484375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.46484375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.53125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.46484375" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
@@ -3416,7 +3438,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
@@ -3442,7 +3464,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>63</v>
       </c>
@@ -3454,7 +3476,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>101</v>
       </c>
@@ -3475,7 +3497,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>101</v>
       </c>
@@ -3496,7 +3518,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>101</v>
       </c>
@@ -3517,7 +3539,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>101</v>
       </c>
@@ -3538,7 +3560,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>101</v>
       </c>
@@ -3559,7 +3581,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>101</v>
       </c>
@@ -3580,7 +3602,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>101</v>
       </c>
@@ -3601,7 +3623,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>101</v>
       </c>
@@ -3622,7 +3644,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>101</v>
       </c>
@@ -3643,7 +3665,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:52" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>101</v>
       </c>
@@ -3664,7 +3686,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:52" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
       <c r="B18" s="47"/>
       <c r="C18" s="47" t="s">
         <v>47</v>
@@ -3719,7 +3741,7 @@
       <c r="AY18"/>
       <c r="AZ18"/>
     </row>
-    <row r="19" spans="2:52" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
       <c r="C19" s="10" t="s">
         <v>64</v>
       </c>
@@ -3776,7 +3798,7 @@
       <c r="AY19"/>
       <c r="AZ19"/>
     </row>
-    <row r="20" spans="2:52" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
       <c r="K20" s="29" t="s">
         <v>102</v>
       </c>
@@ -3822,7 +3844,7 @@
       <c r="AY20"/>
       <c r="AZ20"/>
     </row>
-    <row r="21" spans="2:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K21" s="55" t="s">
         <v>121</v>
       </c>
@@ -3870,7 +3892,7 @@
       <c r="AY21"/>
       <c r="AZ21"/>
     </row>
-    <row r="22" spans="2:52" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:52" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K22" s="30" t="s">
         <v>122</v>
       </c>
@@ -3918,7 +3940,7 @@
       <c r="AY22"/>
       <c r="AZ22"/>
     </row>
-    <row r="23" spans="2:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K23" s="32"/>
       <c r="L23" s="33">
         <v>2010</v>
@@ -4044,7 +4066,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="24" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:52" x14ac:dyDescent="0.35">
       <c r="K24" s="35" t="s">
         <v>104</v>
       </c>
@@ -4212,7 +4234,7 @@
         <v>1.896949318128919</v>
       </c>
     </row>
-    <row r="25" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:52" x14ac:dyDescent="0.35">
       <c r="K25" s="35" t="s">
         <v>105</v>
       </c>
@@ -4381,7 +4403,7 @@
         <v>1.6842224782533921</v>
       </c>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:52" x14ac:dyDescent="0.35">
       <c r="K26" s="61" t="s">
         <v>139</v>
       </c>
@@ -4509,7 +4531,7 @@
         <v>1.8000000000000002E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:52" x14ac:dyDescent="0.35">
       <c r="K27" s="37" t="s">
         <v>123</v>
       </c>
@@ -4637,7 +4659,7 @@
         <v>7.4539999999999997</v>
       </c>
     </row>
-    <row r="28" spans="2:52" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:52" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K28" s="42" t="s">
         <v>106</v>
       </c>
@@ -4806,7 +4828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K29" s="44" t="s">
         <v>154</v>
       </c>
@@ -4852,7 +4874,7 @@
       <c r="AY29"/>
       <c r="AZ29"/>
     </row>
-    <row r="30" spans="2:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K30" s="56"/>
       <c r="L30"/>
       <c r="M30"/>
@@ -4896,7 +4918,7 @@
       <c r="AY30"/>
       <c r="AZ30"/>
     </row>
-    <row r="31" spans="2:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K31" s="57" t="s">
         <v>107</v>
       </c>
@@ -4942,7 +4964,7 @@
       <c r="AY31"/>
       <c r="AZ31"/>
     </row>
-    <row r="32" spans="2:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K32" s="58">
         <v>41767</v>
       </c>
@@ -4992,7 +5014,7 @@
       <c r="AY32"/>
       <c r="AZ32"/>
     </row>
-    <row r="33" spans="11:91" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K33" s="58">
         <v>42102</v>
       </c>
@@ -5042,7 +5064,7 @@
       <c r="AY33" s="45"/>
       <c r="AZ33"/>
     </row>
-    <row r="34" spans="11:91" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K34" s="64">
         <v>42702</v>
       </c>
@@ -5053,7 +5075,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="11:91" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
       <c r="K35" s="73">
         <v>44351</v>
       </c>
@@ -5144,7 +5166,7 @@
       <c r="CL35" s="65"/>
       <c r="CM35" s="66"/>
     </row>
-    <row r="36" spans="11:91" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
       <c r="L36" s="62"/>
       <c r="M36" s="62"/>
       <c r="N36" s="62"/>
@@ -5187,22 +5209,22 @@
       <c r="AY36" s="62"/>
       <c r="AZ36" s="63"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C52" s="10"/>
       <c r="E52" s="17"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53"/>
       <c r="C53" s="10"/>
       <c r="E53" s="17"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58"/>
       <c r="E58" s="9"/>
     </row>
@@ -5226,22 +5248,22 @@
       <selection activeCell="L48" sqref="K48:L49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L2" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="12:16" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="12:16" ht="13.15" x14ac:dyDescent="0.35">
       <c r="L3" s="13" t="s">
         <v>34</v>
       </c>
@@ -5258,7 +5280,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L4" t="s">
         <v>52</v>
       </c>
@@ -5275,7 +5297,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L5" t="s">
         <v>53</v>
       </c>
@@ -5292,7 +5314,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L6" t="s">
         <v>54</v>
       </c>
@@ -5323,19 +5345,19 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.1328125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.46484375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="10" width="11.88671875" customWidth="1"/>
+    <col min="8" max="10" width="11.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -5343,7 +5365,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
@@ -5353,7 +5375,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
@@ -5362,12 +5384,12 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
@@ -5387,7 +5409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="15" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Added the new region MAR
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{46F39D87-D6B9-40D1-9326-C41307F19AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{746BD033-5960-43A8-BD8C-D1F20A120AE8}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{46F39D87-D6B9-40D1-9326-C41307F19AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{928A7A32-A780-4BFB-ACD6-03FC83D64A6C}"/>
   <bookViews>
-    <workbookView xWindow="3218" yWindow="3218" windowWidth="16875" windowHeight="10522" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="22" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="164">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -679,6 +679,21 @@
   </si>
   <si>
     <t>DKISL3</t>
+  </si>
+  <si>
+    <t>DANISLBH</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>DANISL1</t>
+  </si>
+  <si>
+    <t>DANISL2</t>
+  </si>
+  <si>
+    <t>DANISL3</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1217,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1332,6 +1347,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="16" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="5x indented GHG Textfiels" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1949,8 +1967,8 @@
         <v>118</v>
       </c>
       <c r="D5" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!K24),COLUMN(Constants!K24),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!K28),COLUMN(Constants!K28),4,1)</f>
-        <v>K24:K28</v>
+        <f>ADDRESS(ROW(Constants!P24),COLUMN(Constants!P24),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!P28),COLUMN(Constants!P28),4,1)</f>
+        <v>P24:P28</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>142</v>
@@ -1985,8 +2003,8 @@
         <v>118</v>
       </c>
       <c r="D7" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!C8),COLUMN(Constants!C8),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!K14),COLUMN(Constants!K14),4,1)</f>
-        <v>C8:K14</v>
+        <f>ADDRESS(ROW(Constants!C8),COLUMN(Constants!C8),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!P14),COLUMN(Constants!P14),4,1)</f>
+        <v>C8:P14</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>133</v>
@@ -2020,8 +2038,8 @@
         <v>118</v>
       </c>
       <c r="D9" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!K20),COLUMN(Constants!K20),4,1)</f>
-        <v>K20</v>
+        <f>ADDRESS(ROW(Constants!P20),COLUMN(Constants!P20),4,1)</f>
+        <v>P20</v>
       </c>
       <c r="E9" s="50" t="s">
         <v>127</v>
@@ -2149,7 +2167,7 @@
   <dimension ref="A3:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2341,7 +2359,9 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="76" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
@@ -2505,7 +2525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:E53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -3403,10 +3423,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="B3:CM58"/>
+  <dimension ref="B3:CR58"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F28" sqref="F25:F28"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3416,29 +3436,30 @@
     <col min="3" max="3" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.1328125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="6.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.86328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.53125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.46484375" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.1328125" style="8"/>
+    <col min="6" max="10" width="9.46484375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="6.46484375" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.86328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.46484375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.53125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.46484375" style="8" customWidth="1"/>
+    <col min="17" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="P5" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
@@ -3451,20 +3472,35 @@
       <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" s="77" t="s">
+        <v>163</v>
+      </c>
+      <c r="J6" s="77" t="s">
+        <v>160</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="L6" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="P6" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>63</v>
       </c>
@@ -3472,221 +3508,276 @@
       <c r="E7" s="10">
         <v>2020</v>
       </c>
-      <c r="K7" s="69" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="P7" s="69" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>101</v>
       </c>
       <c r="D8"/>
       <c r="E8" s="46">
-        <f>1/L25</f>
+        <f>1/Q25</f>
         <v>1.1263056648526228</v>
       </c>
-      <c r="G8" s="8" t="str">
-        <f t="shared" ref="G8:G15" si="0">K8</f>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="L8" s="8" t="str">
+        <f t="shared" ref="L8:L15" si="0">P8</f>
         <v>MKr10</v>
       </c>
-      <c r="H8" s="8" t="str">
-        <f>$K$7</f>
+      <c r="M8" s="8" t="str">
+        <f>$P$7</f>
         <v>MKr20</v>
       </c>
-      <c r="K8" s="60" t="s">
+      <c r="P8" s="60" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>101</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="46">
-        <f>1/M25</f>
+        <f>1/R25</f>
         <v>1.0988347949781687</v>
       </c>
-      <c r="G9" s="8" t="str">
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="L9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>MKr11</v>
       </c>
-      <c r="H9" s="8" t="str">
-        <f t="shared" ref="H9:H17" si="1">$K$7</f>
+      <c r="M9" s="8" t="str">
+        <f t="shared" ref="M9:M17" si="1">$P$7</f>
         <v>MKr20</v>
       </c>
-      <c r="K9" s="60" t="s">
+      <c r="P9" s="60" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>101</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="46">
-        <f>1/N25</f>
+        <f>1/S25</f>
         <v>1.074129809362824</v>
       </c>
-      <c r="G10" s="8" t="str">
-        <f>K10</f>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="L10" s="8" t="str">
+        <f>P10</f>
         <v>MKr12</v>
       </c>
-      <c r="H10" s="8" t="str">
+      <c r="M10" s="8" t="str">
         <f t="shared" si="1"/>
         <v>MKr20</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="P10" s="60" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>101</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="46">
-        <f>1/O25</f>
+        <f>1/T25</f>
         <v>1.0489548919558829</v>
       </c>
-      <c r="G11" s="8" t="str">
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="L11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>MKr13</v>
       </c>
-      <c r="H11" s="8" t="str">
+      <c r="M11" s="8" t="str">
         <f t="shared" si="1"/>
         <v>MKr20</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="P11" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>101</v>
       </c>
       <c r="D12"/>
       <c r="E12" s="46">
-        <f>1/P25</f>
+        <f>1/U25</f>
         <v>1.0406298531308362</v>
       </c>
-      <c r="G12" s="8" t="str">
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="L12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>MKr14</v>
       </c>
-      <c r="H12" s="8" t="str">
+      <c r="M12" s="8" t="str">
         <f t="shared" si="1"/>
         <v>MKr20</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="P12" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>101</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="46">
-        <f>1/Q25</f>
+        <f>1/V25</f>
         <v>1.0344233132513281</v>
       </c>
-      <c r="G13" s="8" t="str">
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="L13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>MKr15</v>
       </c>
-      <c r="H13" s="8" t="str">
+      <c r="M13" s="8" t="str">
         <f t="shared" si="1"/>
         <v>MKr20</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="P13" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>101</v>
       </c>
       <c r="D14"/>
       <c r="E14" s="46">
-        <f>1/R25</f>
+        <f>1/W25</f>
         <v>1.0303021048320002</v>
       </c>
-      <c r="G14" s="8" t="str">
-        <f>K14</f>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="L14" s="8" t="str">
+        <f>P14</f>
         <v>MKr16</v>
       </c>
-      <c r="H14" s="8" t="str">
+      <c r="M14" s="8" t="str">
         <f t="shared" si="1"/>
         <v>MKr20</v>
       </c>
-      <c r="K14" s="60" t="s">
+      <c r="P14" s="60" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>101</v>
       </c>
       <c r="D15"/>
       <c r="E15" s="46">
-        <f>1/S25</f>
+        <f>1/X25</f>
         <v>1.0292728320000002</v>
       </c>
-      <c r="G15" s="8" t="str">
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="L15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>MKr17</v>
       </c>
-      <c r="H15" s="8" t="str">
+      <c r="M15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>MKr20</v>
       </c>
-      <c r="K15" s="60" t="s">
+      <c r="P15" s="60" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>101</v>
       </c>
       <c r="D16"/>
       <c r="E16" s="46">
-        <f>1/T25</f>
+        <f>1/Y25</f>
         <v>1.0160640000000001</v>
       </c>
-      <c r="G16" s="8" t="str">
-        <f>K16</f>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="L16" s="8" t="str">
+        <f>P16</f>
         <v>MKr18</v>
       </c>
-      <c r="H16" s="8" t="str">
+      <c r="M16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>MKr20</v>
       </c>
-      <c r="K16" s="60" t="s">
+      <c r="P16" s="60" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="2:52" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:57" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>101</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="46">
-        <f>1/U25</f>
+        <f>1/Z25</f>
         <v>1.008</v>
       </c>
-      <c r="G17" s="8" t="str">
-        <f>K17</f>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="L17" s="8" t="str">
+        <f>P17</f>
         <v>MKr19</v>
       </c>
-      <c r="H17" s="8" t="str">
+      <c r="M17" s="8" t="str">
         <f t="shared" si="1"/>
         <v>MKr20</v>
       </c>
-      <c r="K17" s="60" t="s">
+      <c r="P17" s="60" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:57" ht="19.5" x14ac:dyDescent="0.6">
       <c r="B18" s="47"/>
       <c r="C18" s="47" t="s">
         <v>47</v>
@@ -3695,15 +3786,15 @@
       <c r="E18" s="49">
         <v>0.1</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="K18" s="29"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="P18" s="29"/>
       <c r="Q18"/>
       <c r="R18"/>
       <c r="S18"/>
@@ -3740,8 +3831,13 @@
       <c r="AX18"/>
       <c r="AY18"/>
       <c r="AZ18"/>
-    </row>
-    <row r="19" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BD18"/>
+      <c r="BE18"/>
+    </row>
+    <row r="19" spans="2:57" ht="19.5" x14ac:dyDescent="0.6">
       <c r="C19" s="10" t="s">
         <v>64</v>
       </c>
@@ -3752,15 +3848,25 @@
         <f>1-0.07</f>
         <v>0.92999999999999994</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="17">
+        <v>1</v>
+      </c>
+      <c r="G19" s="17">
+        <v>1</v>
+      </c>
+      <c r="H19" s="17">
+        <v>1</v>
+      </c>
+      <c r="I19" s="17">
+        <v>1</v>
+      </c>
+      <c r="J19" s="17">
+        <v>1</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="K19" s="29"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
+      <c r="P19" s="29"/>
       <c r="Q19"/>
       <c r="R19"/>
       <c r="S19"/>
@@ -3797,16 +3903,16 @@
       <c r="AX19"/>
       <c r="AY19"/>
       <c r="AZ19"/>
-    </row>
-    <row r="20" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="K20" s="29" t="s">
+      <c r="BA19"/>
+      <c r="BB19"/>
+      <c r="BC19"/>
+      <c r="BD19"/>
+      <c r="BE19"/>
+    </row>
+    <row r="20" spans="2:57" ht="19.5" x14ac:dyDescent="0.6">
+      <c r="P20" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
-      <c r="P20"/>
       <c r="Q20"/>
       <c r="R20"/>
       <c r="S20"/>
@@ -3843,19 +3949,19 @@
       <c r="AX20"/>
       <c r="AY20"/>
       <c r="AZ20"/>
-    </row>
-    <row r="21" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K21" s="55" t="s">
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+    </row>
+    <row r="21" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P21" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="L21">
+      <c r="Q21">
         <v>2020</v>
       </c>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
       <c r="R21"/>
       <c r="S21"/>
       <c r="T21"/>
@@ -3891,36 +3997,36 @@
       <c r="AX21"/>
       <c r="AY21"/>
       <c r="AZ21"/>
-    </row>
-    <row r="22" spans="2:52" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K22" s="30" t="s">
+      <c r="BA21"/>
+      <c r="BB21"/>
+      <c r="BC21"/>
+      <c r="BD21"/>
+      <c r="BE21"/>
+    </row>
+    <row r="22" spans="2:57" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P22" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
       <c r="U22" s="31"/>
       <c r="V22" s="31"/>
       <c r="W22" s="31"/>
-      <c r="X22"/>
-      <c r="Y22"/>
-      <c r="Z22"/>
-      <c r="AA22"/>
-      <c r="AB22"/>
-      <c r="AC22" t="s">
-        <v>103</v>
-      </c>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31"/>
+      <c r="AC22"/>
       <c r="AD22"/>
       <c r="AE22"/>
       <c r="AF22"/>
       <c r="AG22"/>
-      <c r="AH22"/>
+      <c r="AH22" t="s">
+        <v>103</v>
+      </c>
       <c r="AI22"/>
       <c r="AJ22"/>
       <c r="AK22"/>
@@ -3939,530 +4045,520 @@
       <c r="AX22"/>
       <c r="AY22"/>
       <c r="AZ22"/>
-    </row>
-    <row r="23" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K23" s="32"/>
-      <c r="L23" s="33">
+      <c r="BA22"/>
+      <c r="BB22"/>
+      <c r="BC22"/>
+      <c r="BD22"/>
+      <c r="BE22"/>
+    </row>
+    <row r="23" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P23" s="32"/>
+      <c r="Q23" s="33">
         <v>2010</v>
       </c>
-      <c r="M23" s="33">
+      <c r="R23" s="33">
         <v>2011</v>
       </c>
-      <c r="N23" s="33">
+      <c r="S23" s="33">
         <v>2012</v>
       </c>
-      <c r="O23" s="33">
+      <c r="T23" s="33">
         <v>2013</v>
       </c>
-      <c r="P23" s="33">
+      <c r="U23" s="33">
         <v>2014</v>
       </c>
-      <c r="Q23" s="33">
+      <c r="V23" s="33">
         <v>2015</v>
       </c>
-      <c r="R23" s="33">
+      <c r="W23" s="33">
         <v>2016</v>
       </c>
-      <c r="S23" s="33">
+      <c r="X23" s="33">
         <v>2017</v>
       </c>
-      <c r="T23" s="33">
+      <c r="Y23" s="33">
         <v>2018</v>
       </c>
-      <c r="U23" s="33">
+      <c r="Z23" s="33">
         <v>2019</v>
       </c>
-      <c r="V23" s="33">
+      <c r="AA23" s="33">
         <v>2020</v>
       </c>
-      <c r="W23" s="33">
+      <c r="AB23" s="33">
         <v>2021</v>
       </c>
-      <c r="X23" s="33">
+      <c r="AC23" s="33">
         <v>2022</v>
       </c>
-      <c r="Y23" s="33">
+      <c r="AD23" s="33">
         <v>2023</v>
       </c>
-      <c r="Z23" s="33">
+      <c r="AE23" s="33">
         <v>2024</v>
       </c>
-      <c r="AA23" s="33">
+      <c r="AF23" s="33">
         <v>2025</v>
       </c>
-      <c r="AB23" s="33">
+      <c r="AG23" s="33">
         <v>2026</v>
       </c>
-      <c r="AC23" s="33">
+      <c r="AH23" s="33">
         <v>2027</v>
       </c>
-      <c r="AD23" s="33">
+      <c r="AI23" s="33">
         <v>2028</v>
       </c>
-      <c r="AE23" s="33">
+      <c r="AJ23" s="33">
         <v>2029</v>
       </c>
-      <c r="AF23" s="33">
+      <c r="AK23" s="33">
         <v>2030</v>
       </c>
-      <c r="AG23" s="33">
+      <c r="AL23" s="33">
         <v>2031</v>
       </c>
-      <c r="AH23" s="33">
+      <c r="AM23" s="33">
         <v>2032</v>
       </c>
-      <c r="AI23" s="33">
+      <c r="AN23" s="33">
         <v>2033</v>
       </c>
-      <c r="AJ23" s="33">
+      <c r="AO23" s="33">
         <v>2034</v>
       </c>
-      <c r="AK23" s="33">
+      <c r="AP23" s="33">
         <v>2035</v>
       </c>
-      <c r="AL23" s="33">
+      <c r="AQ23" s="33">
         <v>2036</v>
       </c>
-      <c r="AM23" s="33">
+      <c r="AR23" s="33">
         <v>2037</v>
       </c>
-      <c r="AN23" s="33">
+      <c r="AS23" s="33">
         <v>2038</v>
       </c>
-      <c r="AO23" s="33">
+      <c r="AT23" s="33">
         <v>2039</v>
       </c>
-      <c r="AP23" s="33">
+      <c r="AU23" s="33">
         <v>2040</v>
       </c>
-      <c r="AQ23" s="33">
+      <c r="AV23" s="33">
         <v>2041</v>
       </c>
-      <c r="AR23" s="33">
+      <c r="AW23" s="33">
         <v>2042</v>
       </c>
-      <c r="AS23" s="33">
+      <c r="AX23" s="33">
         <v>2043</v>
       </c>
-      <c r="AT23" s="33">
+      <c r="AY23" s="33">
         <v>2044</v>
       </c>
-      <c r="AU23" s="33">
+      <c r="AZ23" s="33">
         <v>2045</v>
       </c>
-      <c r="AV23" s="33">
+      <c r="BA23" s="33">
         <v>2046</v>
       </c>
-      <c r="AW23" s="33">
+      <c r="BB23" s="33">
         <v>2047</v>
       </c>
-      <c r="AX23" s="33">
+      <c r="BC23" s="33">
         <v>2048</v>
       </c>
-      <c r="AY23" s="33">
+      <c r="BD23" s="33">
         <v>2049</v>
       </c>
-      <c r="AZ23" s="34">
+      <c r="BE23" s="34">
         <v>2050</v>
       </c>
     </row>
-    <row r="24" spans="2:52" x14ac:dyDescent="0.35">
-      <c r="K24" s="35" t="s">
+    <row r="24" spans="2:57" x14ac:dyDescent="0.35">
+      <c r="P24" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="L24" s="36">
-        <v>1</v>
-      </c>
-      <c r="M24" s="36">
-        <f>L24*(L26)+L24</f>
+      <c r="Q24" s="36">
+        <v>1</v>
+      </c>
+      <c r="R24" s="36">
+        <f>Q24*(Q26)+Q24</f>
         <v>1.0249999999999999</v>
       </c>
-      <c r="N24" s="36">
-        <f t="shared" ref="N24:AZ24" si="2">M24*(M26)+M24</f>
+      <c r="S24" s="36">
+        <f t="shared" ref="S24:BE24" si="2">R24*(R26)+R24</f>
         <v>1.0485749999999998</v>
       </c>
-      <c r="O24" s="36">
+      <c r="T24" s="36">
         <f t="shared" si="2"/>
         <v>1.0737407999999997</v>
       </c>
-      <c r="P24" s="36">
+      <c r="U24" s="36">
         <f t="shared" si="2"/>
         <v>1.0823307263999997</v>
       </c>
-      <c r="Q24" s="36">
+      <c r="V24" s="36">
         <f t="shared" si="2"/>
         <v>1.0888247107583997</v>
       </c>
-      <c r="R24" s="36">
+      <c r="W24" s="36">
         <f t="shared" si="2"/>
         <v>1.0931800096014332</v>
       </c>
-      <c r="S24" s="36">
+      <c r="X24" s="36">
         <f t="shared" si="2"/>
         <v>1.0942731896110347</v>
       </c>
-      <c r="T24" s="36">
+      <c r="Y24" s="36">
         <f t="shared" si="2"/>
         <v>1.1084987410759781</v>
       </c>
-      <c r="U24" s="36">
+      <c r="Z24" s="36">
         <f t="shared" si="2"/>
         <v>1.1173667310045861</v>
       </c>
-      <c r="V24" s="36">
+      <c r="AA24" s="36">
         <f t="shared" si="2"/>
         <v>1.1263056648526228</v>
       </c>
-      <c r="W24" s="36">
+      <c r="AB24" s="36">
         <f t="shared" si="2"/>
         <v>1.1296845818471808</v>
       </c>
-      <c r="X24" s="36">
+      <c r="AC24" s="36">
         <f t="shared" si="2"/>
         <v>1.143240796829347</v>
       </c>
-      <c r="Y24" s="36">
+      <c r="AD24" s="36">
         <f t="shared" si="2"/>
         <v>1.1603894087817872</v>
       </c>
-      <c r="Z24" s="36">
+      <c r="AE24" s="36">
         <f t="shared" si="2"/>
         <v>1.1801160287310777</v>
       </c>
-      <c r="AA24" s="36">
+      <c r="AF24" s="36">
         <f t="shared" si="2"/>
         <v>1.201358117248237</v>
       </c>
-      <c r="AB24" s="36">
+      <c r="AG24" s="36">
         <f t="shared" si="2"/>
         <v>1.2217812052414572</v>
       </c>
-      <c r="AC24" s="36">
+      <c r="AH24" s="36">
         <f t="shared" si="2"/>
         <v>1.2437732669358035</v>
       </c>
-      <c r="AD24" s="36">
+      <c r="AI24" s="36">
         <f t="shared" si="2"/>
         <v>1.2649174124737121</v>
       </c>
-      <c r="AE24" s="36">
+      <c r="AJ24" s="36">
         <f t="shared" si="2"/>
         <v>1.2876859258982389</v>
       </c>
-      <c r="AF24" s="36">
+      <c r="AK24" s="36">
         <f t="shared" si="2"/>
         <v>1.3108642725644073</v>
       </c>
-      <c r="AG24" s="36">
+      <c r="AL24" s="36">
         <f t="shared" si="2"/>
         <v>1.3331489651980022</v>
       </c>
-      <c r="AH24" s="36">
+      <c r="AM24" s="36">
         <f t="shared" si="2"/>
         <v>1.3584787955367643</v>
       </c>
-      <c r="AI24" s="36">
+      <c r="AN24" s="36">
         <f t="shared" si="2"/>
         <v>1.3829314138564262</v>
       </c>
-      <c r="AJ24" s="36">
+      <c r="AO24" s="36">
         <f t="shared" si="2"/>
         <v>1.4092071107196982</v>
       </c>
-      <c r="AK24" s="36">
+      <c r="AP24" s="36">
         <f t="shared" si="2"/>
         <v>1.4345728387126528</v>
       </c>
-      <c r="AL24" s="36">
+      <c r="AQ24" s="36">
         <f t="shared" si="2"/>
         <v>1.4603951498094805</v>
       </c>
-      <c r="AM24" s="36">
+      <c r="AR24" s="36">
         <f t="shared" si="2"/>
         <v>1.4896030528056701</v>
       </c>
-      <c r="AN24" s="36">
+      <c r="AS24" s="36">
         <f t="shared" si="2"/>
         <v>1.5179055108089778</v>
       </c>
-      <c r="AO24" s="36">
+      <c r="AT24" s="36">
         <f t="shared" si="2"/>
         <v>1.5467457155143485</v>
       </c>
-      <c r="AP24" s="36">
+      <c r="AU24" s="36">
         <f t="shared" si="2"/>
         <v>1.576133884109121</v>
       </c>
-      <c r="AQ24" s="36">
+      <c r="AV24" s="36">
         <f t="shared" si="2"/>
         <v>1.6060804279071943</v>
       </c>
-      <c r="AR24" s="36">
+      <c r="AW24" s="36">
         <f t="shared" si="2"/>
         <v>1.636595956037431</v>
       </c>
-      <c r="AS24" s="36">
+      <c r="AX24" s="36">
         <f t="shared" si="2"/>
         <v>1.6660546832461047</v>
       </c>
-      <c r="AT24" s="36">
+      <c r="AY24" s="36">
         <f t="shared" si="2"/>
         <v>1.6977097222277808</v>
       </c>
-      <c r="AU24" s="36">
+      <c r="AZ24" s="36">
         <f t="shared" si="2"/>
         <v>1.7299662069501087</v>
       </c>
-      <c r="AV24" s="36">
+      <c r="BA24" s="36">
         <f t="shared" si="2"/>
         <v>1.7611055986752107</v>
       </c>
-      <c r="AW24" s="36">
+      <c r="BB24" s="36">
         <f t="shared" si="2"/>
         <v>1.7945666050500397</v>
       </c>
-      <c r="AX24" s="36">
+      <c r="BC24" s="36">
         <f t="shared" si="2"/>
         <v>1.8268688039409404</v>
       </c>
-      <c r="AY24" s="36">
+      <c r="BD24" s="36">
         <f t="shared" si="2"/>
         <v>1.8615793112158183</v>
       </c>
-      <c r="AZ24" s="36">
+      <c r="BE24" s="36">
         <f t="shared" si="2"/>
         <v>1.896949318128919</v>
       </c>
     </row>
-    <row r="25" spans="2:52" x14ac:dyDescent="0.35">
-      <c r="K25" s="35" t="s">
+    <row r="25" spans="2:57" x14ac:dyDescent="0.35">
+      <c r="P25" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="L25" s="36">
-        <f>L24/HLOOKUP($L$21,$L$23:$AZ$24,2,FALSE)</f>
+      <c r="Q25" s="36">
+        <f>Q24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
         <v>0.88785844838208294</v>
       </c>
-      <c r="M25" s="36">
-        <f t="shared" ref="M25:AZ25" si="3">M24/HLOOKUP($L$21,$L$23:$AZ$24,2,FALSE)</f>
+      <c r="R25" s="36">
+        <f t="shared" ref="R25:BE25" si="3">R24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
         <v>0.91005490959163493</v>
       </c>
-      <c r="N25" s="36">
+      <c r="S25" s="36">
         <f t="shared" si="3"/>
         <v>0.93098617251224236</v>
       </c>
-      <c r="O25" s="36">
+      <c r="T25" s="36">
         <f t="shared" si="3"/>
         <v>0.95332984065253612</v>
       </c>
-      <c r="P25" s="36">
+      <c r="U25" s="36">
         <f t="shared" si="3"/>
         <v>0.96095647937775641</v>
       </c>
-      <c r="Q25" s="36">
+      <c r="V25" s="36">
         <f t="shared" si="3"/>
         <v>0.96672221825402294</v>
       </c>
-      <c r="R25" s="36">
+      <c r="W25" s="36">
         <f t="shared" si="3"/>
         <v>0.97058910712703905</v>
       </c>
-      <c r="S25" s="36">
+      <c r="X25" s="36">
         <f t="shared" si="3"/>
         <v>0.97155969623416605</v>
       </c>
-      <c r="T25" s="36">
+      <c r="Y25" s="36">
         <f t="shared" si="3"/>
         <v>0.98418997228521021</v>
       </c>
-      <c r="U25" s="36">
+      <c r="Z25" s="36">
         <f t="shared" si="3"/>
         <v>0.99206349206349198</v>
       </c>
-      <c r="V25" s="36">
-        <f>V24/HLOOKUP($L$21,$L$23:$AZ$24,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="W25" s="36">
+      <c r="AA25" s="36">
+        <f>AA24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AB25" s="36">
         <f t="shared" si="3"/>
         <v>1.0030000000000001</v>
       </c>
-      <c r="X25" s="36">
+      <c r="AC25" s="36">
         <f t="shared" si="3"/>
         <v>1.015036</v>
       </c>
-      <c r="Y25" s="36">
+      <c r="AD25" s="36">
         <f t="shared" si="3"/>
         <v>1.0302615400000001</v>
       </c>
-      <c r="Z25" s="36">
+      <c r="AE25" s="36">
         <f t="shared" si="3"/>
         <v>1.0477759861800002</v>
       </c>
-      <c r="AA25" s="36">
+      <c r="AF25" s="36">
         <f t="shared" si="3"/>
         <v>1.0666359539312402</v>
       </c>
-      <c r="AB25" s="36">
+      <c r="AG25" s="36">
         <f t="shared" si="3"/>
         <v>1.0847687651480713</v>
       </c>
-      <c r="AC25" s="36">
+      <c r="AH25" s="36">
         <f t="shared" si="3"/>
         <v>1.1042946029207368</v>
       </c>
-      <c r="AD25" s="36">
+      <c r="AI25" s="36">
         <f t="shared" si="3"/>
         <v>1.1230676111703892</v>
       </c>
-      <c r="AE25" s="36">
+      <c r="AJ25" s="36">
         <f t="shared" si="3"/>
         <v>1.1432828281714562</v>
       </c>
-      <c r="AF25" s="36">
+      <c r="AK25" s="36">
         <f t="shared" si="3"/>
         <v>1.1638619190785424</v>
       </c>
-      <c r="AG25" s="36">
+      <c r="AL25" s="36">
         <f t="shared" si="3"/>
         <v>1.1836475717028776</v>
       </c>
-      <c r="AH25" s="36">
+      <c r="AM25" s="36">
         <f t="shared" si="3"/>
         <v>1.2061368755652324</v>
       </c>
-      <c r="AI25" s="36">
+      <c r="AN25" s="36">
         <f t="shared" si="3"/>
         <v>1.2278473393254066</v>
       </c>
-      <c r="AJ25" s="36">
+      <c r="AO25" s="36">
         <f t="shared" si="3"/>
         <v>1.2511764387725892</v>
       </c>
-      <c r="AK25" s="36">
+      <c r="AP25" s="36">
         <f t="shared" si="3"/>
         <v>1.2736976146704959</v>
       </c>
-      <c r="AL25" s="36">
+      <c r="AQ25" s="36">
         <f t="shared" si="3"/>
         <v>1.2966241717345648</v>
       </c>
-      <c r="AM25" s="36">
+      <c r="AR25" s="36">
         <f t="shared" si="3"/>
         <v>1.322556655169256</v>
       </c>
-      <c r="AN25" s="36">
+      <c r="AS25" s="36">
         <f t="shared" si="3"/>
         <v>1.3476852316174721</v>
       </c>
-      <c r="AO25" s="36">
+      <c r="AT25" s="36">
         <f t="shared" si="3"/>
         <v>1.373291251018204</v>
       </c>
-      <c r="AP25" s="36">
+      <c r="AU25" s="36">
         <f t="shared" si="3"/>
         <v>1.3993837847875499</v>
       </c>
-      <c r="AQ25" s="36">
+      <c r="AV25" s="36">
         <f t="shared" si="3"/>
         <v>1.4259720766985133</v>
       </c>
-      <c r="AR25" s="36">
+      <c r="AW25" s="36">
         <f t="shared" si="3"/>
         <v>1.4530655461557851</v>
       </c>
-      <c r="AS25" s="36">
+      <c r="AX25" s="36">
         <f t="shared" si="3"/>
         <v>1.479220725986589</v>
       </c>
-      <c r="AT25" s="36">
+      <c r="AY25" s="36">
         <f t="shared" si="3"/>
         <v>1.5073259197803344</v>
       </c>
-      <c r="AU25" s="36">
+      <c r="AZ25" s="36">
         <f t="shared" si="3"/>
         <v>1.5359651122561608</v>
       </c>
-      <c r="AV25" s="36">
+      <c r="BA25" s="36">
         <f t="shared" si="3"/>
         <v>1.5636124842767718</v>
       </c>
-      <c r="AW25" s="36">
+      <c r="BB25" s="36">
         <f t="shared" si="3"/>
         <v>1.5933211214780305</v>
       </c>
-      <c r="AX25" s="36">
+      <c r="BC25" s="36">
         <f t="shared" si="3"/>
         <v>1.6220009016646351</v>
       </c>
-      <c r="AY25" s="36">
+      <c r="BD25" s="36">
         <f t="shared" si="3"/>
         <v>1.652818918796263</v>
       </c>
-      <c r="AZ25" s="36">
+      <c r="BE25" s="36">
         <f t="shared" si="3"/>
         <v>1.6842224782533921</v>
       </c>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.35">
-      <c r="K26" s="61" t="s">
+    <row r="26" spans="2:57" x14ac:dyDescent="0.35">
+      <c r="P26" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="L26" s="38">
+      <c r="Q26" s="38">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M26" s="38">
+      <c r="R26" s="38">
         <v>2.3E-2</v>
       </c>
-      <c r="N26" s="38">
+      <c r="S26" s="38">
         <v>2.4E-2</v>
-      </c>
-      <c r="O26" s="38">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="P26" s="38">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="Q26" s="38">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="R26" s="38">
-        <v>1E-3</v>
-      </c>
-      <c r="S26" s="38">
-        <v>1.3000000000000001E-2</v>
       </c>
       <c r="T26" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="U26" s="38">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="V26" s="38">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="W26" s="38">
+        <v>1E-3</v>
+      </c>
+      <c r="X26" s="38">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="Y26" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="V26" s="38">
+      <c r="Z26" s="38">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AA26" s="38">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="W26" s="38">
+      <c r="AB26" s="38">
         <v>1.2E-2</v>
       </c>
-      <c r="X26" s="38">
+      <c r="AC26" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y26" s="38">
+      <c r="AD26" s="38">
         <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="Z26" s="38">
-        <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AA26" s="38">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="AB26" s="38">
-        <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AC26" s="38">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="AD26" s="38">
-        <v>1.8000000000000002E-2</v>
       </c>
       <c r="AE26" s="38">
         <v>1.8000000000000002E-2</v>
@@ -4471,40 +4567,40 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="AG26" s="38">
-        <v>1.9E-2</v>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="AH26" s="38">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AI26" s="38">
         <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AI26" s="38">
-        <v>1.9E-2</v>
       </c>
       <c r="AJ26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="AK26" s="38">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AL26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AM26" s="38">
         <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AL26" s="38">
-        <v>0.02</v>
-      </c>
-      <c r="AM26" s="38">
-        <v>1.9E-2</v>
       </c>
       <c r="AN26" s="38">
         <v>1.9E-2</v>
       </c>
       <c r="AO26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="AP26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="AQ26" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="AR26" s="38">
         <v>1.9E-2</v>
-      </c>
-      <c r="AP26" s="38">
-        <v>1.9E-2</v>
-      </c>
-      <c r="AQ26" s="38">
-        <v>1.9E-2</v>
-      </c>
-      <c r="AR26" s="38">
-        <v>1.8000000000000002E-2</v>
       </c>
       <c r="AS26" s="38">
         <v>1.9E-2</v>
@@ -4513,7 +4609,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="AU26" s="38">
-        <v>1.8000000000000002E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AV26" s="38">
         <v>1.9E-2</v>
@@ -4530,28 +4626,28 @@
       <c r="AZ26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
-    </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.35">
-      <c r="K27" s="37" t="s">
+      <c r="BA26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BB26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="BC26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BD26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BE26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:57" x14ac:dyDescent="0.35">
+      <c r="P27" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="L27" s="39">
+      <c r="Q27" s="39">
         <v>7.4470000000000001</v>
-      </c>
-      <c r="M27" s="39">
-        <v>7.4539999999999997</v>
-      </c>
-      <c r="N27" s="39">
-        <v>7.4539999999999997</v>
-      </c>
-      <c r="O27" s="39">
-        <v>7.4539999999999997</v>
-      </c>
-      <c r="P27" s="40">
-        <v>7.4539999999999997</v>
-      </c>
-      <c r="Q27" s="39">
-        <v>7.4539999999999997</v>
       </c>
       <c r="R27" s="39">
         <v>7.4539999999999997</v>
@@ -4562,7 +4658,7 @@
       <c r="T27" s="39">
         <v>7.4539999999999997</v>
       </c>
-      <c r="U27" s="39">
+      <c r="U27" s="40">
         <v>7.4539999999999997</v>
       </c>
       <c r="V27" s="39">
@@ -4655,49 +4751,44 @@
       <c r="AY27" s="39">
         <v>7.4539999999999997</v>
       </c>
-      <c r="AZ27" s="41">
+      <c r="AZ27" s="39">
         <v>7.4539999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="2:52" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K28" s="42" t="s">
+      <c r="BA27" s="39">
+        <v>7.4539999999999997</v>
+      </c>
+      <c r="BB27" s="39">
+        <v>7.4539999999999997</v>
+      </c>
+      <c r="BC27" s="39">
+        <v>7.4539999999999997</v>
+      </c>
+      <c r="BD27" s="39">
+        <v>7.4539999999999997</v>
+      </c>
+      <c r="BE27" s="41">
+        <v>7.4539999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:57" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P28" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="L28" s="43" t="str">
-        <f>L35</f>
+      <c r="Q28" s="43" t="str">
+        <f>Q35</f>
         <v>MBS</v>
       </c>
-      <c r="M28" s="43" t="str">
-        <f t="shared" ref="M28:AZ28" si="4">M35</f>
+      <c r="R28" s="43" t="str">
+        <f t="shared" ref="R28:BE28" si="4">R35</f>
         <v>Opdateret med DK2025</v>
-      </c>
-      <c r="N28" s="43">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="43" t="str">
-        <f t="shared" si="4"/>
-        <v>https://fm.dk/udgivelser/2020/august/dk2025-en-groen-retfaerdig-og-ansvarlig-genopretning-af-dansk-oekonomi/</v>
-      </c>
-      <c r="P28" s="43">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="43">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="43">
-        <f t="shared" si="4"/>
-        <v>0</v>
       </c>
       <c r="S28" s="43">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T28" s="43">
+      <c r="T28" s="43" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>https://fm.dk/udgivelser/2020/august/dk2025-en-groen-retfaerdig-og-ansvarlig-genopretning-af-dansk-oekonomi/</v>
       </c>
       <c r="U28" s="43">
         <f t="shared" si="4"/>
@@ -4827,16 +4918,31 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K29" s="44" t="s">
+      <c r="BA28" s="43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="BB28" s="43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="BC28" s="43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="BD28" s="43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="BE28" s="43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P29" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
@@ -4844,11 +4950,11 @@
       <c r="U29" s="7"/>
       <c r="V29" s="7"/>
       <c r="W29" s="7"/>
-      <c r="X29"/>
-      <c r="Y29"/>
-      <c r="Z29"/>
-      <c r="AA29"/>
-      <c r="AB29"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
       <c r="AC29"/>
       <c r="AD29"/>
       <c r="AE29"/>
@@ -4873,14 +4979,14 @@
       <c r="AX29"/>
       <c r="AY29"/>
       <c r="AZ29"/>
-    </row>
-    <row r="30" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K30" s="56"/>
-      <c r="L30"/>
-      <c r="M30"/>
-      <c r="N30"/>
-      <c r="O30"/>
-      <c r="P30"/>
+      <c r="BA29"/>
+      <c r="BB29"/>
+      <c r="BC29"/>
+      <c r="BD29"/>
+      <c r="BE29"/>
+    </row>
+    <row r="30" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P30" s="56"/>
       <c r="Q30"/>
       <c r="R30"/>
       <c r="S30"/>
@@ -4917,16 +5023,16 @@
       <c r="AX30"/>
       <c r="AY30"/>
       <c r="AZ30"/>
-    </row>
-    <row r="31" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K31" s="57" t="s">
+      <c r="BA30"/>
+      <c r="BB30"/>
+      <c r="BC30"/>
+      <c r="BD30"/>
+      <c r="BE30"/>
+    </row>
+    <row r="31" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P31" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
       <c r="Q31"/>
       <c r="R31"/>
       <c r="S31"/>
@@ -4963,22 +5069,22 @@
       <c r="AX31"/>
       <c r="AY31"/>
       <c r="AZ31"/>
-    </row>
-    <row r="32" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K32" s="58">
+      <c r="BA31"/>
+      <c r="BB31"/>
+      <c r="BC31"/>
+      <c r="BD31"/>
+      <c r="BE31"/>
+    </row>
+    <row r="32" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P32" s="58">
         <v>41767</v>
       </c>
-      <c r="L32" s="59" t="s">
+      <c r="Q32" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="M32" s="59" t="s">
+      <c r="R32" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
       <c r="S32"/>
       <c r="T32"/>
       <c r="U32"/>
@@ -5013,23 +5119,23 @@
       <c r="AX32"/>
       <c r="AY32"/>
       <c r="AZ32"/>
-    </row>
-    <row r="33" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K33" s="58">
+      <c r="BA32"/>
+      <c r="BB32"/>
+      <c r="BC32"/>
+      <c r="BD32"/>
+      <c r="BE32"/>
+    </row>
+    <row r="33" spans="16:96" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P33" s="58">
         <v>42102</v>
       </c>
-      <c r="L33" s="59" t="s">
+      <c r="Q33" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="M33" s="59" t="s">
+      <c r="R33" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="N33"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
+      <c r="S33"/>
       <c r="T33" s="45"/>
       <c r="U33" s="45"/>
       <c r="V33" s="45"/>
@@ -5062,38 +5168,38 @@
       <c r="AW33" s="45"/>
       <c r="AX33" s="45"/>
       <c r="AY33" s="45"/>
-      <c r="AZ33"/>
-    </row>
-    <row r="34" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K34" s="64">
+      <c r="AZ33" s="45"/>
+      <c r="BA33" s="45"/>
+      <c r="BB33" s="45"/>
+      <c r="BC33" s="45"/>
+      <c r="BD33" s="45"/>
+      <c r="BE33"/>
+    </row>
+    <row r="34" spans="16:96" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P34" s="64">
         <v>42702</v>
       </c>
-      <c r="L34" s="69" t="s">
+      <c r="Q34" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="M34" s="59" t="s">
+      <c r="R34" s="59" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K35" s="73">
+    <row r="35" spans="16:96" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="P35" s="73">
         <v>44351</v>
       </c>
-      <c r="L35" s="74" t="s">
+      <c r="Q35" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="M35" s="74" t="s">
+      <c r="R35" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="N35" s="67"/>
-      <c r="O35" s="75" t="s">
+      <c r="S35" s="67"/>
+      <c r="T35" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="P35" s="67"/>
-      <c r="Q35" s="67"/>
-      <c r="R35" s="67"/>
-      <c r="S35" s="67"/>
-      <c r="T35" s="67"/>
       <c r="U35" s="67"/>
       <c r="V35" s="67"/>
       <c r="W35" s="67"/>
@@ -5125,12 +5231,12 @@
       <c r="AW35" s="67"/>
       <c r="AX35" s="67"/>
       <c r="AY35" s="67"/>
-      <c r="AZ35" s="68"/>
-      <c r="BA35" s="65"/>
-      <c r="BB35" s="65"/>
-      <c r="BC35" s="65"/>
-      <c r="BD35" s="65"/>
-      <c r="BE35" s="65"/>
+      <c r="AZ35" s="67"/>
+      <c r="BA35" s="67"/>
+      <c r="BB35" s="67"/>
+      <c r="BC35" s="67"/>
+      <c r="BD35" s="67"/>
+      <c r="BE35" s="68"/>
       <c r="BF35" s="65"/>
       <c r="BG35" s="65"/>
       <c r="BH35" s="65"/>
@@ -5164,14 +5270,14 @@
       <c r="CJ35" s="65"/>
       <c r="CK35" s="65"/>
       <c r="CL35" s="65"/>
-      <c r="CM35" s="66"/>
-    </row>
-    <row r="36" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="L36" s="62"/>
-      <c r="M36" s="62"/>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
+      <c r="CM35" s="65"/>
+      <c r="CN35" s="65"/>
+      <c r="CO35" s="65"/>
+      <c r="CP35" s="65"/>
+      <c r="CQ35" s="65"/>
+      <c r="CR35" s="66"/>
+    </row>
+    <row r="36" spans="16:96" ht="14.25" x14ac:dyDescent="0.45">
       <c r="Q36" s="62"/>
       <c r="R36" s="62"/>
       <c r="S36" s="62"/>
@@ -5207,31 +5313,61 @@
       <c r="AW36" s="62"/>
       <c r="AX36" s="62"/>
       <c r="AY36" s="62"/>
-      <c r="AZ36" s="63"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="AZ36" s="62"/>
+      <c r="BA36" s="62"/>
+      <c r="BB36" s="62"/>
+      <c r="BC36" s="62"/>
+      <c r="BD36" s="62"/>
+      <c r="BE36" s="63"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C52" s="10"/>
       <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B53"/>
       <c r="C53" s="10"/>
       <c r="E53" s="17"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E56" s="9"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E57" s="9"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B58"/>
       <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="O35" r:id="rId1" xr:uid="{2A5C4B4A-D7D5-4EDE-B99F-9E5AC5DB0C93}"/>
+    <hyperlink ref="T35" r:id="rId1" xr:uid="{2A5C4B4A-D7D5-4EDE-B99F-9E5AC5DB0C93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Change tranmission network loss - all regions are divided into the smaller regions
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{46F39D87-D6B9-40D1-9326-C41307F19AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{928A7A32-A780-4BFB-ACD6-03FC83D64A6C}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{46F39D87-D6B9-40D1-9326-C41307F19AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4721AD15-5F09-4DE6-AE0C-9C7D194B3B90}"/>
   <bookViews>
-    <workbookView xWindow="46470" yWindow="1470" windowWidth="20760" windowHeight="12180" tabRatio="853" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="16875" windowHeight="10522" tabRatio="853" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="22" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="164">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -700,9 +700,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -1217,7 +1218,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1350,6 +1351,8 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="5x indented GHG Textfiels" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1979,8 +1982,8 @@
         <v>118</v>
       </c>
       <c r="D5" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!P24),COLUMN(Constants!P24),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!P28),COLUMN(Constants!P28),4,1)</f>
-        <v>P24:P28</v>
+        <f>ADDRESS(ROW(Constants!Q24),COLUMN(Constants!Q24),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!Q28),COLUMN(Constants!Q28),4,1)</f>
+        <v>Q24:Q28</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>142</v>
@@ -2015,8 +2018,8 @@
         <v>118</v>
       </c>
       <c r="D7" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!C8),COLUMN(Constants!C8),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!P14),COLUMN(Constants!P14),4,1)</f>
-        <v>C8:P14</v>
+        <f>ADDRESS(ROW(Constants!C8),COLUMN(Constants!C8),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!Q14),COLUMN(Constants!Q14),4,1)</f>
+        <v>C8:Q14</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>133</v>
@@ -2050,8 +2053,8 @@
         <v>118</v>
       </c>
       <c r="D9" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!P20),COLUMN(Constants!P20),4,1)</f>
-        <v>P20</v>
+        <f>ADDRESS(ROW(Constants!Q20),COLUMN(Constants!Q20),4,1)</f>
+        <v>Q20</v>
       </c>
       <c r="E9" s="50" t="s">
         <v>127</v>
@@ -3435,10 +3438,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="B3:CR58"/>
+  <dimension ref="B3:CS58"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3448,30 +3451,30 @@
     <col min="3" max="3" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.1328125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9.46484375" style="8" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="6.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.86328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.53125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.46484375" style="8" customWidth="1"/>
-    <col min="17" max="16384" width="9.1328125" style="8"/>
+    <col min="6" max="11" width="9.46484375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="6.46484375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.86328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.46484375" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.53125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.46484375" style="8" customWidth="1"/>
+    <col min="18" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:17" ht="15" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="Q5" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:17" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
@@ -3482,37 +3485,40 @@
         <v>23</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="F6" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="77" t="s">
         <v>159</v>
       </c>
-      <c r="G6" s="77" t="s">
+      <c r="H6" s="77" t="s">
         <v>161</v>
       </c>
-      <c r="H6" s="77" t="s">
+      <c r="I6" s="77" t="s">
         <v>162</v>
       </c>
-      <c r="I6" s="77" t="s">
+      <c r="J6" s="77" t="s">
         <v>163</v>
       </c>
-      <c r="J6" s="77" t="s">
+      <c r="K6" s="77" t="s">
         <v>160</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="L6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="N6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="P6" s="13" t="s">
+      <c r="Q6" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>63</v>
       </c>
@@ -3520,276 +3526,485 @@
       <c r="E7" s="10">
         <v>2020</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="P7" s="69" t="s">
+      <c r="F7" s="79">
+        <f>E7</f>
+        <v>2020</v>
+      </c>
+      <c r="G7" s="79">
+        <f>F7</f>
+        <v>2020</v>
+      </c>
+      <c r="H7" s="79">
+        <f t="shared" ref="H7:K7" si="0">G7</f>
+        <v>2020</v>
+      </c>
+      <c r="I7" s="79">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="J7" s="79">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="K7" s="79">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="Q7" s="69" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>101</v>
       </c>
       <c r="D8"/>
       <c r="E8" s="46">
-        <f>1/Q25</f>
+        <f>1/R25</f>
         <v>1.1263056648526228</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="L8" s="8" t="str">
-        <f t="shared" ref="L8:L15" si="0">P8</f>
+      <c r="F8" s="46">
+        <f t="shared" ref="F8:G8" si="1">E8</f>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="G8" s="46">
+        <f t="shared" si="1"/>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="H8" s="46">
+        <f t="shared" ref="H8:K8" si="2">G8</f>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="I8" s="46">
+        <f t="shared" si="2"/>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="J8" s="46">
+        <f t="shared" si="2"/>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="K8" s="46">
+        <f t="shared" si="2"/>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="M8" s="8" t="str">
+        <f t="shared" ref="M8:M15" si="3">Q8</f>
         <v>MKr10</v>
       </c>
-      <c r="M8" s="8" t="str">
-        <f>$P$7</f>
+      <c r="N8" s="8" t="str">
+        <f>$Q$7</f>
         <v>MKr20</v>
       </c>
-      <c r="P8" s="60" t="s">
+      <c r="Q8" s="60" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>101</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="46">
-        <f>1/R25</f>
+        <f>1/S25</f>
         <v>1.0988347949781687</v>
       </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="L9" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F9" s="46">
+        <f t="shared" ref="F9:G9" si="4">E9</f>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="G9" s="46">
+        <f t="shared" si="4"/>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="H9" s="46">
+        <f t="shared" ref="H9:K9" si="5">G9</f>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="I9" s="46">
+        <f t="shared" si="5"/>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="J9" s="46">
+        <f t="shared" si="5"/>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="K9" s="46">
+        <f t="shared" si="5"/>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="M9" s="8" t="str">
+        <f t="shared" si="3"/>
         <v>MKr11</v>
       </c>
-      <c r="M9" s="8" t="str">
-        <f t="shared" ref="M9:M17" si="1">$P$7</f>
+      <c r="N9" s="8" t="str">
+        <f t="shared" ref="N9:N17" si="6">$Q$7</f>
         <v>MKr20</v>
       </c>
-      <c r="P9" s="60" t="s">
+      <c r="Q9" s="60" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>101</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="46">
-        <f>1/S25</f>
+        <f>1/T25</f>
         <v>1.074129809362824</v>
       </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="L10" s="8" t="str">
-        <f>P10</f>
+      <c r="F10" s="46">
+        <f t="shared" ref="F10:G10" si="7">E10</f>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="G10" s="46">
+        <f t="shared" si="7"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="H10" s="46">
+        <f t="shared" ref="H10:K10" si="8">G10</f>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="I10" s="46">
+        <f t="shared" si="8"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="J10" s="46">
+        <f t="shared" si="8"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="K10" s="46">
+        <f t="shared" si="8"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="M10" s="8" t="str">
+        <f>Q10</f>
         <v>MKr12</v>
       </c>
-      <c r="M10" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="N10" s="8" t="str">
+        <f t="shared" si="6"/>
         <v>MKr20</v>
       </c>
-      <c r="P10" s="60" t="s">
+      <c r="Q10" s="60" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>101</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="46">
-        <f>1/T25</f>
+        <f>1/U25</f>
         <v>1.0489548919558829</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="L11" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F11" s="46">
+        <f t="shared" ref="F11:G11" si="9">E11</f>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="G11" s="46">
+        <f t="shared" si="9"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="H11" s="46">
+        <f t="shared" ref="H11:K11" si="10">G11</f>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="I11" s="46">
+        <f t="shared" si="10"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="J11" s="46">
+        <f t="shared" si="10"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="K11" s="46">
+        <f t="shared" si="10"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="M11" s="8" t="str">
+        <f t="shared" si="3"/>
         <v>MKr13</v>
       </c>
-      <c r="M11" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="N11" s="8" t="str">
+        <f t="shared" si="6"/>
         <v>MKr20</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="Q11" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>101</v>
       </c>
       <c r="D12"/>
       <c r="E12" s="46">
-        <f>1/U25</f>
+        <f>1/V25</f>
         <v>1.0406298531308362</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="L12" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F12" s="46">
+        <f t="shared" ref="F12:G12" si="11">E12</f>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="G12" s="46">
+        <f t="shared" si="11"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="H12" s="46">
+        <f t="shared" ref="H12:K12" si="12">G12</f>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="I12" s="46">
+        <f t="shared" si="12"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="J12" s="46">
+        <f t="shared" si="12"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="K12" s="46">
+        <f t="shared" si="12"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="M12" s="8" t="str">
+        <f t="shared" si="3"/>
         <v>MKr14</v>
       </c>
-      <c r="M12" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="N12" s="8" t="str">
+        <f t="shared" si="6"/>
         <v>MKr20</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="Q12" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>101</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="46">
-        <f>1/V25</f>
+        <f>1/W25</f>
         <v>1.0344233132513281</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="L13" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F13" s="46">
+        <f t="shared" ref="F13:G13" si="13">E13</f>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="G13" s="46">
+        <f t="shared" si="13"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="H13" s="46">
+        <f t="shared" ref="H13:K13" si="14">G13</f>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="I13" s="46">
+        <f t="shared" si="14"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="J13" s="46">
+        <f t="shared" si="14"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="K13" s="46">
+        <f t="shared" si="14"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="M13" s="8" t="str">
+        <f t="shared" si="3"/>
         <v>MKr15</v>
       </c>
-      <c r="M13" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="N13" s="8" t="str">
+        <f t="shared" si="6"/>
         <v>MKr20</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="Q13" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>101</v>
       </c>
       <c r="D14"/>
       <c r="E14" s="46">
-        <f>1/W25</f>
+        <f>1/X25</f>
         <v>1.0303021048320002</v>
       </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="L14" s="8" t="str">
-        <f>P14</f>
+      <c r="F14" s="46">
+        <f t="shared" ref="F14:G14" si="15">E14</f>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="G14" s="46">
+        <f t="shared" si="15"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="H14" s="46">
+        <f t="shared" ref="H14:K14" si="16">G14</f>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="I14" s="46">
+        <f t="shared" si="16"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="J14" s="46">
+        <f t="shared" si="16"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="K14" s="46">
+        <f t="shared" si="16"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="M14" s="8" t="str">
+        <f>Q14</f>
         <v>MKr16</v>
       </c>
-      <c r="M14" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="N14" s="8" t="str">
+        <f t="shared" si="6"/>
         <v>MKr20</v>
       </c>
-      <c r="P14" s="60" t="s">
+      <c r="Q14" s="60" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>101</v>
       </c>
       <c r="D15"/>
       <c r="E15" s="46">
-        <f>1/X25</f>
+        <f>1/Y25</f>
         <v>1.0292728320000002</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="L15" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F15" s="46">
+        <f t="shared" ref="F15:G15" si="17">E15</f>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="G15" s="46">
+        <f t="shared" si="17"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="H15" s="46">
+        <f t="shared" ref="H15:K15" si="18">G15</f>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="I15" s="46">
+        <f t="shared" si="18"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="J15" s="46">
+        <f t="shared" si="18"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="K15" s="46">
+        <f t="shared" si="18"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="M15" s="8" t="str">
+        <f t="shared" si="3"/>
         <v>MKr17</v>
       </c>
-      <c r="M15" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="N15" s="8" t="str">
+        <f t="shared" si="6"/>
         <v>MKr20</v>
       </c>
-      <c r="P15" s="60" t="s">
+      <c r="Q15" s="60" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>101</v>
       </c>
       <c r="D16"/>
       <c r="E16" s="46">
-        <f>1/Y25</f>
+        <f>1/Z25</f>
         <v>1.0160640000000001</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="L16" s="8" t="str">
-        <f>P16</f>
+      <c r="F16" s="46">
+        <f t="shared" ref="F16:G16" si="19">E16</f>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="G16" s="46">
+        <f t="shared" si="19"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="H16" s="46">
+        <f t="shared" ref="H16:K16" si="20">G16</f>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="I16" s="46">
+        <f t="shared" si="20"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="J16" s="46">
+        <f t="shared" si="20"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="K16" s="46">
+        <f t="shared" si="20"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="M16" s="8" t="str">
+        <f>Q16</f>
         <v>MKr18</v>
       </c>
-      <c r="M16" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="N16" s="8" t="str">
+        <f t="shared" si="6"/>
         <v>MKr20</v>
       </c>
-      <c r="P16" s="60" t="s">
+      <c r="Q16" s="60" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="2:57" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:58" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>101</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="46">
-        <f>1/Z25</f>
+        <f>1/AA25</f>
         <v>1.008</v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="L17" s="8" t="str">
-        <f>P17</f>
+      <c r="F17" s="46">
+        <f t="shared" ref="F17:G17" si="21">E17</f>
+        <v>1.008</v>
+      </c>
+      <c r="G17" s="46">
+        <f t="shared" si="21"/>
+        <v>1.008</v>
+      </c>
+      <c r="H17" s="46">
+        <f t="shared" ref="H17:K17" si="22">G17</f>
+        <v>1.008</v>
+      </c>
+      <c r="I17" s="46">
+        <f t="shared" si="22"/>
+        <v>1.008</v>
+      </c>
+      <c r="J17" s="46">
+        <f t="shared" si="22"/>
+        <v>1.008</v>
+      </c>
+      <c r="K17" s="46">
+        <f t="shared" si="22"/>
+        <v>1.008</v>
+      </c>
+      <c r="M17" s="8" t="str">
+        <f>Q17</f>
         <v>MKr19</v>
       </c>
-      <c r="M17" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="N17" s="8" t="str">
+        <f t="shared" si="6"/>
         <v>MKr20</v>
       </c>
-      <c r="P17" s="60" t="s">
+      <c r="Q17" s="60" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:57" ht="19.5" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:58" ht="19.5" x14ac:dyDescent="0.6">
       <c r="B18" s="47"/>
       <c r="C18" s="47" t="s">
         <v>47</v>
@@ -3798,16 +4013,28 @@
       <c r="E18" s="49">
         <v>0.1</v>
       </c>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="47"/>
+      <c r="F18" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="49">
+        <v>0.1</v>
+      </c>
       <c r="L18" s="47"/>
       <c r="M18" s="47"/>
-      <c r="P18" s="29"/>
-      <c r="Q18"/>
+      <c r="N18" s="47"/>
+      <c r="Q18" s="29"/>
       <c r="R18"/>
       <c r="S18"/>
       <c r="T18"/>
@@ -3848,8 +4075,9 @@
       <c r="BC18"/>
       <c r="BD18"/>
       <c r="BE18"/>
-    </row>
-    <row r="19" spans="2:57" ht="19.5" x14ac:dyDescent="0.6">
+      <c r="BF18"/>
+    </row>
+    <row r="19" spans="2:58" ht="19.5" x14ac:dyDescent="0.6">
       <c r="C19" s="10" t="s">
         <v>64</v>
       </c>
@@ -3860,26 +4088,28 @@
         <f>1-0.07</f>
         <v>0.92999999999999994</v>
       </c>
-      <c r="F19" s="17">
-        <v>1</v>
-      </c>
-      <c r="G19" s="17">
-        <v>1</v>
-      </c>
-      <c r="H19" s="17">
-        <v>1</v>
-      </c>
-      <c r="I19" s="17">
-        <v>1</v>
-      </c>
-      <c r="J19" s="17">
-        <v>1</v>
-      </c>
-      <c r="K19" s="8" t="s">
+      <c r="F19" s="78">
+        <v>1</v>
+      </c>
+      <c r="G19" s="78">
+        <v>1</v>
+      </c>
+      <c r="H19" s="78">
+        <v>1</v>
+      </c>
+      <c r="I19" s="78">
+        <v>1</v>
+      </c>
+      <c r="J19" s="78">
+        <v>1</v>
+      </c>
+      <c r="K19" s="78">
+        <v>1</v>
+      </c>
+      <c r="L19" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="P19" s="29"/>
-      <c r="Q19"/>
+      <c r="Q19" s="29"/>
       <c r="R19"/>
       <c r="S19"/>
       <c r="T19"/>
@@ -3920,12 +4150,12 @@
       <c r="BC19"/>
       <c r="BD19"/>
       <c r="BE19"/>
-    </row>
-    <row r="20" spans="2:57" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="P20" s="29" t="s">
+      <c r="BF19"/>
+    </row>
+    <row r="20" spans="2:58" ht="19.5" x14ac:dyDescent="0.6">
+      <c r="Q20" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="Q20"/>
       <c r="R20"/>
       <c r="S20"/>
       <c r="T20"/>
@@ -3966,15 +4196,15 @@
       <c r="BC20"/>
       <c r="BD20"/>
       <c r="BE20"/>
-    </row>
-    <row r="21" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P21" s="55" t="s">
+      <c r="BF20"/>
+    </row>
+    <row r="21" spans="2:58" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q21" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>2020</v>
       </c>
-      <c r="R21"/>
       <c r="S21"/>
       <c r="T21"/>
       <c r="U21"/>
@@ -4014,16 +4244,16 @@
       <c r="BC21"/>
       <c r="BD21"/>
       <c r="BE21"/>
-    </row>
-    <row r="22" spans="2:57" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P22" s="30" t="s">
+      <c r="BF21"/>
+    </row>
+    <row r="22" spans="2:58" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q22" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
-      <c r="U22" s="31"/>
+      <c r="U22" s="7"/>
       <c r="V22" s="31"/>
       <c r="W22" s="31"/>
       <c r="X22" s="31"/>
@@ -4031,15 +4261,15 @@
       <c r="Z22" s="31"/>
       <c r="AA22" s="31"/>
       <c r="AB22" s="31"/>
-      <c r="AC22"/>
+      <c r="AC22" s="31"/>
       <c r="AD22"/>
       <c r="AE22"/>
       <c r="AF22"/>
       <c r="AG22"/>
-      <c r="AH22" t="s">
+      <c r="AH22"/>
+      <c r="AI22" t="s">
         <v>103</v>
       </c>
-      <c r="AI22"/>
       <c r="AJ22"/>
       <c r="AK22"/>
       <c r="AL22"/>
@@ -4062,557 +4292,555 @@
       <c r="BC22"/>
       <c r="BD22"/>
       <c r="BE22"/>
-    </row>
-    <row r="23" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P23" s="32"/>
-      <c r="Q23" s="33">
+      <c r="BF22"/>
+    </row>
+    <row r="23" spans="2:58" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q23" s="32"/>
+      <c r="R23" s="33">
         <v>2010</v>
       </c>
-      <c r="R23" s="33">
+      <c r="S23" s="33">
         <v>2011</v>
       </c>
-      <c r="S23" s="33">
+      <c r="T23" s="33">
         <v>2012</v>
       </c>
-      <c r="T23" s="33">
+      <c r="U23" s="33">
         <v>2013</v>
       </c>
-      <c r="U23" s="33">
+      <c r="V23" s="33">
         <v>2014</v>
       </c>
-      <c r="V23" s="33">
+      <c r="W23" s="33">
         <v>2015</v>
       </c>
-      <c r="W23" s="33">
+      <c r="X23" s="33">
         <v>2016</v>
       </c>
-      <c r="X23" s="33">
+      <c r="Y23" s="33">
         <v>2017</v>
       </c>
-      <c r="Y23" s="33">
+      <c r="Z23" s="33">
         <v>2018</v>
       </c>
-      <c r="Z23" s="33">
+      <c r="AA23" s="33">
         <v>2019</v>
       </c>
-      <c r="AA23" s="33">
+      <c r="AB23" s="33">
         <v>2020</v>
       </c>
-      <c r="AB23" s="33">
+      <c r="AC23" s="33">
         <v>2021</v>
       </c>
-      <c r="AC23" s="33">
+      <c r="AD23" s="33">
         <v>2022</v>
       </c>
-      <c r="AD23" s="33">
+      <c r="AE23" s="33">
         <v>2023</v>
       </c>
-      <c r="AE23" s="33">
+      <c r="AF23" s="33">
         <v>2024</v>
       </c>
-      <c r="AF23" s="33">
+      <c r="AG23" s="33">
         <v>2025</v>
       </c>
-      <c r="AG23" s="33">
+      <c r="AH23" s="33">
         <v>2026</v>
       </c>
-      <c r="AH23" s="33">
+      <c r="AI23" s="33">
         <v>2027</v>
       </c>
-      <c r="AI23" s="33">
+      <c r="AJ23" s="33">
         <v>2028</v>
       </c>
-      <c r="AJ23" s="33">
+      <c r="AK23" s="33">
         <v>2029</v>
       </c>
-      <c r="AK23" s="33">
+      <c r="AL23" s="33">
         <v>2030</v>
       </c>
-      <c r="AL23" s="33">
+      <c r="AM23" s="33">
         <v>2031</v>
       </c>
-      <c r="AM23" s="33">
+      <c r="AN23" s="33">
         <v>2032</v>
       </c>
-      <c r="AN23" s="33">
+      <c r="AO23" s="33">
         <v>2033</v>
       </c>
-      <c r="AO23" s="33">
+      <c r="AP23" s="33">
         <v>2034</v>
       </c>
-      <c r="AP23" s="33">
+      <c r="AQ23" s="33">
         <v>2035</v>
       </c>
-      <c r="AQ23" s="33">
+      <c r="AR23" s="33">
         <v>2036</v>
       </c>
-      <c r="AR23" s="33">
+      <c r="AS23" s="33">
         <v>2037</v>
       </c>
-      <c r="AS23" s="33">
+      <c r="AT23" s="33">
         <v>2038</v>
       </c>
-      <c r="AT23" s="33">
+      <c r="AU23" s="33">
         <v>2039</v>
       </c>
-      <c r="AU23" s="33">
+      <c r="AV23" s="33">
         <v>2040</v>
       </c>
-      <c r="AV23" s="33">
+      <c r="AW23" s="33">
         <v>2041</v>
       </c>
-      <c r="AW23" s="33">
+      <c r="AX23" s="33">
         <v>2042</v>
       </c>
-      <c r="AX23" s="33">
+      <c r="AY23" s="33">
         <v>2043</v>
       </c>
-      <c r="AY23" s="33">
+      <c r="AZ23" s="33">
         <v>2044</v>
       </c>
-      <c r="AZ23" s="33">
+      <c r="BA23" s="33">
         <v>2045</v>
       </c>
-      <c r="BA23" s="33">
+      <c r="BB23" s="33">
         <v>2046</v>
       </c>
-      <c r="BB23" s="33">
+      <c r="BC23" s="33">
         <v>2047</v>
       </c>
-      <c r="BC23" s="33">
+      <c r="BD23" s="33">
         <v>2048</v>
       </c>
-      <c r="BD23" s="33">
+      <c r="BE23" s="33">
         <v>2049</v>
       </c>
-      <c r="BE23" s="34">
+      <c r="BF23" s="34">
         <v>2050</v>
       </c>
     </row>
-    <row r="24" spans="2:57" x14ac:dyDescent="0.35">
-      <c r="P24" s="35" t="s">
+    <row r="24" spans="2:58" x14ac:dyDescent="0.35">
+      <c r="Q24" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="Q24" s="36">
-        <v>1</v>
-      </c>
       <c r="R24" s="36">
-        <f>Q24*(Q26)+Q24</f>
+        <v>1</v>
+      </c>
+      <c r="S24" s="36">
+        <f>R24*(R26)+R24</f>
         <v>1.0249999999999999</v>
       </c>
-      <c r="S24" s="36">
-        <f t="shared" ref="S24:BE24" si="2">R24*(R26)+R24</f>
+      <c r="T24" s="36">
+        <f t="shared" ref="T24:BF24" si="23">S24*(S26)+S24</f>
         <v>1.0485749999999998</v>
       </c>
-      <c r="T24" s="36">
-        <f t="shared" si="2"/>
+      <c r="U24" s="36">
+        <f t="shared" si="23"/>
         <v>1.0737407999999997</v>
       </c>
-      <c r="U24" s="36">
-        <f t="shared" si="2"/>
+      <c r="V24" s="36">
+        <f t="shared" si="23"/>
         <v>1.0823307263999997</v>
       </c>
-      <c r="V24" s="36">
-        <f t="shared" si="2"/>
+      <c r="W24" s="36">
+        <f t="shared" si="23"/>
         <v>1.0888247107583997</v>
       </c>
-      <c r="W24" s="36">
-        <f t="shared" si="2"/>
+      <c r="X24" s="36">
+        <f t="shared" si="23"/>
         <v>1.0931800096014332</v>
       </c>
-      <c r="X24" s="36">
-        <f t="shared" si="2"/>
+      <c r="Y24" s="36">
+        <f t="shared" si="23"/>
         <v>1.0942731896110347</v>
       </c>
-      <c r="Y24" s="36">
-        <f t="shared" si="2"/>
+      <c r="Z24" s="36">
+        <f t="shared" si="23"/>
         <v>1.1084987410759781</v>
       </c>
-      <c r="Z24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AA24" s="36">
+        <f t="shared" si="23"/>
         <v>1.1173667310045861</v>
       </c>
-      <c r="AA24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AB24" s="36">
+        <f t="shared" si="23"/>
         <v>1.1263056648526228</v>
       </c>
-      <c r="AB24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AC24" s="36">
+        <f t="shared" si="23"/>
         <v>1.1296845818471808</v>
       </c>
-      <c r="AC24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AD24" s="36">
+        <f t="shared" si="23"/>
         <v>1.143240796829347</v>
       </c>
-      <c r="AD24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AE24" s="36">
+        <f t="shared" si="23"/>
         <v>1.1603894087817872</v>
       </c>
-      <c r="AE24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AF24" s="36">
+        <f t="shared" si="23"/>
         <v>1.1801160287310777</v>
       </c>
-      <c r="AF24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AG24" s="36">
+        <f t="shared" si="23"/>
         <v>1.201358117248237</v>
       </c>
-      <c r="AG24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AH24" s="36">
+        <f t="shared" si="23"/>
         <v>1.2217812052414572</v>
       </c>
-      <c r="AH24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AI24" s="36">
+        <f t="shared" si="23"/>
         <v>1.2437732669358035</v>
       </c>
-      <c r="AI24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AJ24" s="36">
+        <f t="shared" si="23"/>
         <v>1.2649174124737121</v>
       </c>
-      <c r="AJ24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AK24" s="36">
+        <f t="shared" si="23"/>
         <v>1.2876859258982389</v>
       </c>
-      <c r="AK24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AL24" s="36">
+        <f t="shared" si="23"/>
         <v>1.3108642725644073</v>
       </c>
-      <c r="AL24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AM24" s="36">
+        <f t="shared" si="23"/>
         <v>1.3331489651980022</v>
       </c>
-      <c r="AM24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AN24" s="36">
+        <f t="shared" si="23"/>
         <v>1.3584787955367643</v>
       </c>
-      <c r="AN24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AO24" s="36">
+        <f t="shared" si="23"/>
         <v>1.3829314138564262</v>
       </c>
-      <c r="AO24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AP24" s="36">
+        <f t="shared" si="23"/>
         <v>1.4092071107196982</v>
       </c>
-      <c r="AP24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AQ24" s="36">
+        <f t="shared" si="23"/>
         <v>1.4345728387126528</v>
       </c>
-      <c r="AQ24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AR24" s="36">
+        <f t="shared" si="23"/>
         <v>1.4603951498094805</v>
       </c>
-      <c r="AR24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AS24" s="36">
+        <f t="shared" si="23"/>
         <v>1.4896030528056701</v>
       </c>
-      <c r="AS24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AT24" s="36">
+        <f t="shared" si="23"/>
         <v>1.5179055108089778</v>
       </c>
-      <c r="AT24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AU24" s="36">
+        <f t="shared" si="23"/>
         <v>1.5467457155143485</v>
       </c>
-      <c r="AU24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AV24" s="36">
+        <f t="shared" si="23"/>
         <v>1.576133884109121</v>
       </c>
-      <c r="AV24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AW24" s="36">
+        <f t="shared" si="23"/>
         <v>1.6060804279071943</v>
       </c>
-      <c r="AW24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AX24" s="36">
+        <f t="shared" si="23"/>
         <v>1.636595956037431</v>
       </c>
-      <c r="AX24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AY24" s="36">
+        <f t="shared" si="23"/>
         <v>1.6660546832461047</v>
       </c>
-      <c r="AY24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AZ24" s="36">
+        <f t="shared" si="23"/>
         <v>1.6977097222277808</v>
       </c>
-      <c r="AZ24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BA24" s="36">
+        <f t="shared" si="23"/>
         <v>1.7299662069501087</v>
       </c>
-      <c r="BA24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BB24" s="36">
+        <f t="shared" si="23"/>
         <v>1.7611055986752107</v>
       </c>
-      <c r="BB24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BC24" s="36">
+        <f t="shared" si="23"/>
         <v>1.7945666050500397</v>
       </c>
-      <c r="BC24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BD24" s="36">
+        <f t="shared" si="23"/>
         <v>1.8268688039409404</v>
       </c>
-      <c r="BD24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BE24" s="36">
+        <f t="shared" si="23"/>
         <v>1.8615793112158183</v>
       </c>
-      <c r="BE24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BF24" s="36">
+        <f t="shared" si="23"/>
         <v>1.896949318128919</v>
       </c>
     </row>
-    <row r="25" spans="2:57" x14ac:dyDescent="0.35">
-      <c r="P25" s="35" t="s">
+    <row r="25" spans="2:58" x14ac:dyDescent="0.35">
+      <c r="Q25" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="Q25" s="36">
-        <f>Q24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
+      <c r="R25" s="36">
+        <f>R24/HLOOKUP($R$21,$R$23:$BF$24,2,FALSE)</f>
         <v>0.88785844838208294</v>
       </c>
-      <c r="R25" s="36">
-        <f t="shared" ref="R25:BE25" si="3">R24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
+      <c r="S25" s="36">
+        <f t="shared" ref="S25:BF25" si="24">S24/HLOOKUP($R$21,$R$23:$BF$24,2,FALSE)</f>
         <v>0.91005490959163493</v>
       </c>
-      <c r="S25" s="36">
-        <f t="shared" si="3"/>
+      <c r="T25" s="36">
+        <f t="shared" si="24"/>
         <v>0.93098617251224236</v>
       </c>
-      <c r="T25" s="36">
-        <f t="shared" si="3"/>
+      <c r="U25" s="36">
+        <f t="shared" si="24"/>
         <v>0.95332984065253612</v>
       </c>
-      <c r="U25" s="36">
-        <f t="shared" si="3"/>
+      <c r="V25" s="36">
+        <f t="shared" si="24"/>
         <v>0.96095647937775641</v>
       </c>
-      <c r="V25" s="36">
-        <f t="shared" si="3"/>
+      <c r="W25" s="36">
+        <f t="shared" si="24"/>
         <v>0.96672221825402294</v>
       </c>
-      <c r="W25" s="36">
-        <f t="shared" si="3"/>
+      <c r="X25" s="36">
+        <f t="shared" si="24"/>
         <v>0.97058910712703905</v>
       </c>
-      <c r="X25" s="36">
-        <f t="shared" si="3"/>
+      <c r="Y25" s="36">
+        <f t="shared" si="24"/>
         <v>0.97155969623416605</v>
       </c>
-      <c r="Y25" s="36">
-        <f t="shared" si="3"/>
+      <c r="Z25" s="36">
+        <f t="shared" si="24"/>
         <v>0.98418997228521021</v>
       </c>
-      <c r="Z25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AA25" s="36">
+        <f t="shared" si="24"/>
         <v>0.99206349206349198</v>
       </c>
-      <c r="AA25" s="36">
-        <f>AA24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
-        <v>1</v>
-      </c>
       <c r="AB25" s="36">
-        <f t="shared" si="3"/>
+        <f>AB24/HLOOKUP($R$21,$R$23:$BF$24,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AC25" s="36">
+        <f t="shared" si="24"/>
         <v>1.0030000000000001</v>
       </c>
-      <c r="AC25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AD25" s="36">
+        <f t="shared" si="24"/>
         <v>1.015036</v>
       </c>
-      <c r="AD25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AE25" s="36">
+        <f t="shared" si="24"/>
         <v>1.0302615400000001</v>
       </c>
-      <c r="AE25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AF25" s="36">
+        <f t="shared" si="24"/>
         <v>1.0477759861800002</v>
       </c>
-      <c r="AF25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AG25" s="36">
+        <f t="shared" si="24"/>
         <v>1.0666359539312402</v>
       </c>
-      <c r="AG25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AH25" s="36">
+        <f t="shared" si="24"/>
         <v>1.0847687651480713</v>
       </c>
-      <c r="AH25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AI25" s="36">
+        <f t="shared" si="24"/>
         <v>1.1042946029207368</v>
       </c>
-      <c r="AI25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AJ25" s="36">
+        <f t="shared" si="24"/>
         <v>1.1230676111703892</v>
       </c>
-      <c r="AJ25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AK25" s="36">
+        <f t="shared" si="24"/>
         <v>1.1432828281714562</v>
       </c>
-      <c r="AK25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AL25" s="36">
+        <f t="shared" si="24"/>
         <v>1.1638619190785424</v>
       </c>
-      <c r="AL25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AM25" s="36">
+        <f t="shared" si="24"/>
         <v>1.1836475717028776</v>
       </c>
-      <c r="AM25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AN25" s="36">
+        <f t="shared" si="24"/>
         <v>1.2061368755652324</v>
       </c>
-      <c r="AN25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AO25" s="36">
+        <f t="shared" si="24"/>
         <v>1.2278473393254066</v>
       </c>
-      <c r="AO25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AP25" s="36">
+        <f t="shared" si="24"/>
         <v>1.2511764387725892</v>
       </c>
-      <c r="AP25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AQ25" s="36">
+        <f t="shared" si="24"/>
         <v>1.2736976146704959</v>
       </c>
-      <c r="AQ25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AR25" s="36">
+        <f t="shared" si="24"/>
         <v>1.2966241717345648</v>
       </c>
-      <c r="AR25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AS25" s="36">
+        <f t="shared" si="24"/>
         <v>1.322556655169256</v>
       </c>
-      <c r="AS25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AT25" s="36">
+        <f t="shared" si="24"/>
         <v>1.3476852316174721</v>
       </c>
-      <c r="AT25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AU25" s="36">
+        <f t="shared" si="24"/>
         <v>1.373291251018204</v>
       </c>
-      <c r="AU25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AV25" s="36">
+        <f t="shared" si="24"/>
         <v>1.3993837847875499</v>
       </c>
-      <c r="AV25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AW25" s="36">
+        <f t="shared" si="24"/>
         <v>1.4259720766985133</v>
       </c>
-      <c r="AW25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AX25" s="36">
+        <f t="shared" si="24"/>
         <v>1.4530655461557851</v>
       </c>
-      <c r="AX25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AY25" s="36">
+        <f t="shared" si="24"/>
         <v>1.479220725986589</v>
       </c>
-      <c r="AY25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AZ25" s="36">
+        <f t="shared" si="24"/>
         <v>1.5073259197803344</v>
       </c>
-      <c r="AZ25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BA25" s="36">
+        <f t="shared" si="24"/>
         <v>1.5359651122561608</v>
       </c>
-      <c r="BA25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BB25" s="36">
+        <f t="shared" si="24"/>
         <v>1.5636124842767718</v>
       </c>
-      <c r="BB25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BC25" s="36">
+        <f t="shared" si="24"/>
         <v>1.5933211214780305</v>
       </c>
-      <c r="BC25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BD25" s="36">
+        <f t="shared" si="24"/>
         <v>1.6220009016646351</v>
       </c>
-      <c r="BD25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BE25" s="36">
+        <f t="shared" si="24"/>
         <v>1.652818918796263</v>
       </c>
-      <c r="BE25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BF25" s="36">
+        <f t="shared" si="24"/>
         <v>1.6842224782533921</v>
       </c>
     </row>
-    <row r="26" spans="2:57" x14ac:dyDescent="0.35">
-      <c r="P26" s="61" t="s">
+    <row r="26" spans="2:58" x14ac:dyDescent="0.35">
+      <c r="Q26" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="Q26" s="38">
+      <c r="R26" s="38">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="R26" s="38">
+      <c r="S26" s="38">
         <v>2.3E-2</v>
       </c>
-      <c r="S26" s="38">
+      <c r="T26" s="38">
         <v>2.4E-2</v>
       </c>
-      <c r="T26" s="38">
+      <c r="U26" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="U26" s="38">
+      <c r="V26" s="38">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="V26" s="38">
+      <c r="W26" s="38">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="W26" s="38">
+      <c r="X26" s="38">
         <v>1E-3</v>
       </c>
-      <c r="X26" s="38">
+      <c r="Y26" s="38">
         <v>1.3000000000000001E-2</v>
-      </c>
-      <c r="Y26" s="38">
-        <v>8.0000000000000002E-3</v>
       </c>
       <c r="Z26" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AA26" s="38">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AB26" s="38">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AB26" s="38">
+      <c r="AC26" s="38">
         <v>1.2E-2</v>
       </c>
-      <c r="AC26" s="38">
+      <c r="AD26" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AD26" s="38">
+      <c r="AE26" s="38">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AE26" s="38">
+      <c r="AF26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="AF26" s="38">
+      <c r="AG26" s="38">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AG26" s="38">
+      <c r="AH26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="AH26" s="38">
+      <c r="AI26" s="38">
         <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="AI26" s="38">
-        <v>1.8000000000000002E-2</v>
       </c>
       <c r="AJ26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="AK26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="AL26" s="38">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AL26" s="38">
+      <c r="AM26" s="38">
         <v>1.9E-2</v>
       </c>
-      <c r="AM26" s="38">
+      <c r="AN26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="AN26" s="38">
+      <c r="AO26" s="38">
         <v>1.9E-2</v>
-      </c>
-      <c r="AO26" s="38">
-        <v>1.8000000000000002E-2</v>
       </c>
       <c r="AP26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="AQ26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="AR26" s="38">
         <v>0.02</v>
-      </c>
-      <c r="AR26" s="38">
-        <v>1.9E-2</v>
       </c>
       <c r="AS26" s="38">
         <v>1.9E-2</v>
@@ -4627,42 +4855,42 @@
         <v>1.9E-2</v>
       </c>
       <c r="AW26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AX26" s="38">
         <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AX26" s="38">
-        <v>1.9E-2</v>
       </c>
       <c r="AY26" s="38">
         <v>1.9E-2</v>
       </c>
       <c r="AZ26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BA26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="BA26" s="38">
+      <c r="BB26" s="38">
         <v>1.9E-2</v>
       </c>
-      <c r="BB26" s="38">
+      <c r="BC26" s="38">
         <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="BC26" s="38">
-        <v>1.9E-2</v>
       </c>
       <c r="BD26" s="38">
         <v>1.9E-2</v>
       </c>
       <c r="BE26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BF26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:57" x14ac:dyDescent="0.35">
-      <c r="P27" s="37" t="s">
+    <row r="27" spans="2:58" x14ac:dyDescent="0.35">
+      <c r="Q27" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="Q27" s="39">
+      <c r="R27" s="39">
         <v>7.4470000000000001</v>
-      </c>
-      <c r="R27" s="39">
-        <v>7.4539999999999997</v>
       </c>
       <c r="S27" s="39">
         <v>7.4539999999999997</v>
@@ -4670,10 +4898,10 @@
       <c r="T27" s="39">
         <v>7.4539999999999997</v>
       </c>
-      <c r="U27" s="40">
+      <c r="U27" s="39">
         <v>7.4539999999999997</v>
       </c>
-      <c r="V27" s="39">
+      <c r="V27" s="40">
         <v>7.4539999999999997</v>
       </c>
       <c r="W27" s="39">
@@ -4778,184 +5006,186 @@
       <c r="BD27" s="39">
         <v>7.4539999999999997</v>
       </c>
-      <c r="BE27" s="41">
+      <c r="BE27" s="39">
         <v>7.4539999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="2:57" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P28" s="42" t="s">
+      <c r="BF27" s="41">
+        <v>7.4539999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:58" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q28" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="Q28" s="43" t="str">
-        <f>Q35</f>
+      <c r="R28" s="43" t="str">
+        <f>R35</f>
         <v>MBS</v>
       </c>
-      <c r="R28" s="43" t="str">
-        <f t="shared" ref="R28:BE28" si="4">R35</f>
+      <c r="S28" s="43" t="str">
+        <f t="shared" ref="S28:BF28" si="25">S35</f>
         <v>Opdateret med DK2025</v>
       </c>
-      <c r="S28" s="43">
-        <f t="shared" si="4"/>
+      <c r="T28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="T28" s="43" t="str">
-        <f t="shared" si="4"/>
+      <c r="U28" s="43" t="str">
+        <f t="shared" si="25"/>
         <v>https://fm.dk/udgivelser/2020/august/dk2025-en-groen-retfaerdig-og-ansvarlig-genopretning-af-dansk-oekonomi/</v>
       </c>
-      <c r="U28" s="43">
-        <f t="shared" si="4"/>
+      <c r="V28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="V28" s="43">
-        <f t="shared" si="4"/>
+      <c r="W28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="W28" s="43">
-        <f t="shared" si="4"/>
+      <c r="X28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="X28" s="43">
-        <f t="shared" si="4"/>
+      <c r="Y28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="Y28" s="43">
-        <f t="shared" si="4"/>
+      <c r="Z28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="Z28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AA28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AA28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AB28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AC28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AC28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AD28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AD28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AE28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AE28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AF28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AF28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AG28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AG28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AH28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AH28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AI28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AI28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AJ28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AJ28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AK28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AK28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AL28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AL28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AM28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AM28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AN28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AN28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AO28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AO28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AP28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AP28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AQ28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AQ28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AR28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AR28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AS28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AS28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AT28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AT28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AU28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AU28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AV28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AV28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AW28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AW28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AX28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AX28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AY28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AY28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AZ28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AZ28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BA28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BA28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BB28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BB28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BC28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BC28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BD28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BD28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BE28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="BE28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BF28" s="43">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P29" s="44" t="s">
+    <row r="29" spans="2:58" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q29" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
@@ -4967,7 +5197,7 @@
       <c r="Z29" s="7"/>
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
-      <c r="AC29"/>
+      <c r="AC29" s="7"/>
       <c r="AD29"/>
       <c r="AE29"/>
       <c r="AF29"/>
@@ -4996,10 +5226,10 @@
       <c r="BC29"/>
       <c r="BD29"/>
       <c r="BE29"/>
-    </row>
-    <row r="30" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P30" s="56"/>
-      <c r="Q30"/>
+      <c r="BF29"/>
+    </row>
+    <row r="30" spans="2:58" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q30" s="56"/>
       <c r="R30"/>
       <c r="S30"/>
       <c r="T30"/>
@@ -5040,12 +5270,12 @@
       <c r="BC30"/>
       <c r="BD30"/>
       <c r="BE30"/>
-    </row>
-    <row r="31" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P31" s="57" t="s">
+      <c r="BF30"/>
+    </row>
+    <row r="31" spans="2:58" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q31" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="Q31"/>
       <c r="R31"/>
       <c r="S31"/>
       <c r="T31"/>
@@ -5086,18 +5316,18 @@
       <c r="BC31"/>
       <c r="BD31"/>
       <c r="BE31"/>
-    </row>
-    <row r="32" spans="2:57" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P32" s="58">
+      <c r="BF31"/>
+    </row>
+    <row r="32" spans="2:58" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q32" s="58">
         <v>41767</v>
       </c>
-      <c r="Q32" s="59" t="s">
+      <c r="R32" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="R32" s="59" t="s">
+      <c r="S32" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="S32"/>
       <c r="T32"/>
       <c r="U32"/>
       <c r="V32"/>
@@ -5136,19 +5366,19 @@
       <c r="BC32"/>
       <c r="BD32"/>
       <c r="BE32"/>
-    </row>
-    <row r="33" spans="16:96" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P33" s="58">
+      <c r="BF32"/>
+    </row>
+    <row r="33" spans="17:97" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q33" s="58">
         <v>42102</v>
       </c>
-      <c r="Q33" s="59" t="s">
+      <c r="R33" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="R33" s="59" t="s">
+      <c r="S33" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="S33"/>
-      <c r="T33" s="45"/>
+      <c r="T33"/>
       <c r="U33" s="45"/>
       <c r="V33" s="45"/>
       <c r="W33" s="45"/>
@@ -5185,34 +5415,34 @@
       <c r="BB33" s="45"/>
       <c r="BC33" s="45"/>
       <c r="BD33" s="45"/>
-      <c r="BE33"/>
-    </row>
-    <row r="34" spans="16:96" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P34" s="64">
+      <c r="BE33" s="45"/>
+      <c r="BF33"/>
+    </row>
+    <row r="34" spans="17:97" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q34" s="64">
         <v>42702</v>
       </c>
-      <c r="Q34" s="69" t="s">
+      <c r="R34" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="R34" s="59" t="s">
+      <c r="S34" s="59" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="16:96" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="P35" s="73">
+    <row r="35" spans="17:97" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="Q35" s="73">
         <v>44351</v>
       </c>
-      <c r="Q35" s="74" t="s">
+      <c r="R35" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="R35" s="74" t="s">
+      <c r="S35" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="S35" s="67"/>
-      <c r="T35" s="75" t="s">
+      <c r="T35" s="67"/>
+      <c r="U35" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="U35" s="67"/>
       <c r="V35" s="67"/>
       <c r="W35" s="67"/>
       <c r="X35" s="67"/>
@@ -5248,8 +5478,8 @@
       <c r="BB35" s="67"/>
       <c r="BC35" s="67"/>
       <c r="BD35" s="67"/>
-      <c r="BE35" s="68"/>
-      <c r="BF35" s="65"/>
+      <c r="BE35" s="67"/>
+      <c r="BF35" s="68"/>
       <c r="BG35" s="65"/>
       <c r="BH35" s="65"/>
       <c r="BI35" s="65"/>
@@ -5287,10 +5517,10 @@
       <c r="CO35" s="65"/>
       <c r="CP35" s="65"/>
       <c r="CQ35" s="65"/>
-      <c r="CR35" s="66"/>
-    </row>
-    <row r="36" spans="16:96" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="Q36" s="62"/>
+      <c r="CR35" s="65"/>
+      <c r="CS35" s="66"/>
+    </row>
+    <row r="36" spans="17:97" ht="14.25" x14ac:dyDescent="0.45">
       <c r="R36" s="62"/>
       <c r="S36" s="62"/>
       <c r="T36" s="62"/>
@@ -5330,9 +5560,10 @@
       <c r="BB36" s="62"/>
       <c r="BC36" s="62"/>
       <c r="BD36" s="62"/>
-      <c r="BE36" s="63"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="BE36" s="62"/>
+      <c r="BF36" s="63"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C52" s="10"/>
       <c r="E52" s="17"/>
       <c r="F52" s="17"/>
@@ -5340,8 +5571,9 @@
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
       <c r="J52" s="17"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K52" s="17"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B53"/>
       <c r="C53" s="10"/>
       <c r="E53" s="17"/>
@@ -5350,24 +5582,27 @@
       <c r="H53" s="17"/>
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K53" s="17"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.35">
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K56" s="9"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.35">
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K57" s="9"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B58"/>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
@@ -5375,11 +5610,12 @@
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="T35" r:id="rId1" xr:uid="{2A5C4B4A-D7D5-4EDE-B99F-9E5AC5DB0C93}"/>
+    <hyperlink ref="U35" r:id="rId1" xr:uid="{2A5C4B4A-D7D5-4EDE-B99F-9E5AC5DB0C93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5392,7 +5628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="L2:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L48" sqref="K48:L49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix the transmission losses for the islands in SysSettings.xlsx
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{46F39D87-D6B9-40D1-9326-C41307F19AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{746BD033-5960-43A8-BD8C-D1F20A120AE8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE746CE6-D6AF-435D-A71E-D8047EE5CA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3218" yWindow="3218" windowWidth="16875" windowHeight="10522" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="792" windowWidth="20100" windowHeight="15888" tabRatio="853" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="22" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="159">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1202,7 +1202,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1332,6 +1332,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="16" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="5x indented GHG Textfiels" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1339,8 +1342,9 @@
     <cellStyle name="AggOrange9_CRFReport-template" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="CustomizationCells" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Euro" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8"/>
     <cellStyle name="InputCells" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Link" xfId="17" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
@@ -1349,8 +1353,7 @@
     <cellStyle name="Normal GHG Textfiels Bold" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal GHG-Shade" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Normale_B2020" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Prozent" xfId="14" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="14" builtinId="5"/>
     <cellStyle name="Обычный_CRF2002 (1)" xfId="15" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1565,7 +1568,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1894,16 +1897,16 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.53125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" customWidth="1"/>
-    <col min="4" max="4" width="19.86328125" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
     <col min="5" max="5" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
@@ -1920,7 +1923,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="51">
         <v>42843</v>
       </c>
@@ -1938,7 +1941,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="51">
         <v>42702</v>
       </c>
@@ -1949,14 +1952,14 @@
         <v>118</v>
       </c>
       <c r="D5" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!K24),COLUMN(Constants!K24),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!K28),COLUMN(Constants!K28),4,1)</f>
-        <v>K24:K28</v>
+        <f>ADDRESS(ROW(Constants!P24),COLUMN(Constants!P24),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!P28),COLUMN(Constants!P28),4,1)</f>
+        <v>P24:P28</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="51">
         <v>42604</v>
       </c>
@@ -1974,7 +1977,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="51">
         <v>42549</v>
       </c>
@@ -1985,14 +1988,14 @@
         <v>118</v>
       </c>
       <c r="D7" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!C8),COLUMN(Constants!C8),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!K14),COLUMN(Constants!K14),4,1)</f>
-        <v>C8:K14</v>
+        <f>ADDRESS(ROW(Constants!C8),COLUMN(Constants!C8),4,1)&amp;":"&amp;ADDRESS(ROW(Constants!P14),COLUMN(Constants!P14),4,1)</f>
+        <v>C8:P14</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="51">
         <v>42115</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="51">
         <v>42341</v>
       </c>
@@ -2020,14 +2023,14 @@
         <v>118</v>
       </c>
       <c r="D9" s="50" t="str">
-        <f>ADDRESS(ROW(Constants!K20),COLUMN(Constants!K20),4,1)</f>
-        <v>K20</v>
+        <f>ADDRESS(ROW(Constants!P20),COLUMN(Constants!P20),4,1)</f>
+        <v>P20</v>
       </c>
       <c r="E9" s="50" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="51">
         <v>42311</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51">
         <v>42264</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="51">
         <v>42264</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51">
         <v>42264</v>
       </c>
@@ -2099,7 +2102,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51">
         <v>42264</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51">
         <v>42264</v>
       </c>
@@ -2148,21 +2151,21 @@
   </sheetPr>
   <dimension ref="A3:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.1328125" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="12" t="s">
         <v>10</v>
@@ -2173,7 +2176,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="13" t="s">
         <v>16</v>
@@ -2191,7 +2194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>57</v>
       </c>
@@ -2230,7 +2233,7 @@
       </c>
       <c r="S5" s="20"/>
     </row>
-    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>78</v>
       </c>
@@ -2266,7 +2269,7 @@
       </c>
       <c r="S6" s="20"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="76" t="s">
@@ -2294,7 +2297,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="76" t="s">
@@ -2323,7 +2326,7 @@
       </c>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="76" t="s">
@@ -2331,19 +2334,19 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="76" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2361,7 +2364,7 @@
       <c r="Q12" s="21"/>
       <c r="R12" s="21"/>
     </row>
-    <row r="13" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:19" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2377,7 +2380,7 @@
       <c r="Q13" s="21"/>
       <c r="R13" s="21"/>
     </row>
-    <row r="14" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2387,7 +2390,7 @@
       <c r="Q14" s="21"/>
       <c r="R14" s="21"/>
     </row>
-    <row r="15" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:19" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2397,7 +2400,7 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="21"/>
     </row>
-    <row r="16" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:19" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2407,7 +2410,7 @@
       <c r="Q16" s="21"/>
       <c r="R16" s="21"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2417,7 +2420,7 @@
       <c r="Q17" s="21"/>
       <c r="R17" s="21"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2427,69 +2430,69 @@
       <c r="Q18" s="21"/>
       <c r="R18" s="21"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
     </row>
   </sheetData>
@@ -2509,40 +2512,40 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="70" t="s">
         <v>128</v>
       </c>
@@ -2556,7 +2559,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="18">
         <v>1</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18">
         <v>1</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="18">
         <v>1</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="18">
         <v>1</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="18">
         <v>1</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="18">
         <v>1</v>
       </c>
@@ -2640,7 +2643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="18">
         <v>1</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="18">
         <v>1</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="18">
         <v>1</v>
       </c>
@@ -2682,7 +2685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="18">
         <v>1</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="18">
         <v>1</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="18">
         <v>1</v>
       </c>
@@ -2724,7 +2727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="18">
         <v>1</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <v>1</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="18">
         <v>1</v>
       </c>
@@ -2766,7 +2769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="18">
         <v>1</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="18">
         <v>1</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="18">
         <v>1</v>
       </c>
@@ -2806,7 +2809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="18">
         <v>1</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="18">
         <v>1</v>
       </c>
@@ -2830,7 +2833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="18">
         <v>1</v>
       </c>
@@ -2840,7 +2843,7 @@
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="18">
         <v>1</v>
       </c>
@@ -2850,7 +2853,7 @@
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="18">
         <v>1</v>
       </c>
@@ -2860,7 +2863,7 @@
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="18">
         <v>1</v>
       </c>
@@ -2870,7 +2873,7 @@
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="18">
         <v>1</v>
       </c>
@@ -2880,7 +2883,7 @@
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="18">
         <v>1</v>
       </c>
@@ -2890,7 +2893,7 @@
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="18">
         <v>1</v>
       </c>
@@ -2900,7 +2903,7 @@
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="18">
         <v>1</v>
       </c>
@@ -2910,7 +2913,7 @@
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="18">
         <v>1</v>
       </c>
@@ -2920,7 +2923,7 @@
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="18">
         <v>1</v>
       </c>
@@ -2930,7 +2933,7 @@
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="18">
         <v>1</v>
       </c>
@@ -2938,7 +2941,7 @@
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="18">
         <v>1</v>
       </c>
@@ -2946,7 +2949,7 @@
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="18">
         <v>1</v>
       </c>
@@ -2954,7 +2957,7 @@
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="18">
         <v>1</v>
       </c>
@@ -2962,7 +2965,7 @@
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="18">
         <v>1</v>
       </c>
@@ -2970,7 +2973,7 @@
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="18">
         <v>1</v>
       </c>
@@ -2978,7 +2981,7 @@
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="18">
         <v>1</v>
       </c>
@@ -2986,7 +2989,7 @@
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="18">
         <v>1</v>
       </c>
@@ -2994,7 +2997,7 @@
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="18">
         <v>1</v>
       </c>
@@ -3002,7 +3005,7 @@
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="18">
         <v>1</v>
       </c>
@@ -3010,7 +3013,7 @@
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="18">
         <v>1</v>
       </c>
@@ -3034,20 +3037,20 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.86328125" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>45</v>
       </c>
@@ -3061,19 +3064,19 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="5" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
@@ -3165,7 +3168,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>86</v>
       </c>
@@ -3181,60 +3184,60 @@
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E10" s="7"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E11" s="7"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E12" s="7"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E13" s="7"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E14" s="7"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E15" s="7"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="19" spans="2:16" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
         <v>20</v>
       </c>
@@ -3281,7 +3284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>4</v>
       </c>
@@ -3298,7 +3301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>4</v>
       </c>
@@ -3331,18 +3334,18 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.46484375" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
     <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
         <v>34</v>
       </c>
@@ -3350,7 +3353,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>36</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>37</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
         <v>38</v>
       </c>
@@ -3374,7 +3377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
         <v>39</v>
       </c>
@@ -3382,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
         <v>80</v>
       </c>
@@ -3403,42 +3406,43 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="B3:CM58"/>
+  <dimension ref="B3:CR58"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F28" sqref="F25:F28"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="8"/>
+    <col min="1" max="1" width="9.109375" style="8"/>
     <col min="2" max="2" width="13.6640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="6.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.86328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.53125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.46484375" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.1328125" style="8"/>
+    <col min="4" max="4" width="5.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9.44140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.44140625" style="8" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="P5" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
@@ -3449,22 +3453,37 @@
         <v>23</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="77" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="J6" s="77" t="s">
+        <v>158</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="L6" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="P6" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" s="8" t="s">
         <v>63</v>
       </c>
@@ -3472,221 +3491,441 @@
       <c r="E7" s="10">
         <v>2020</v>
       </c>
-      <c r="K7" s="69" t="s">
+      <c r="F7" s="10">
+        <f>E7</f>
+        <v>2020</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" ref="G7:J7" si="0">F7</f>
+        <v>2020</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="P7" s="69" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>101</v>
       </c>
       <c r="D8"/>
       <c r="E8" s="46">
-        <f>1/L25</f>
+        <f>1/Q25</f>
         <v>1.1263056648526228</v>
       </c>
-      <c r="G8" s="8" t="str">
-        <f t="shared" ref="G8:G15" si="0">K8</f>
+      <c r="F8" s="46">
+        <f>E8</f>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="G8" s="46">
+        <f t="shared" ref="G8:J8" si="1">F8</f>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="H8" s="46">
+        <f t="shared" si="1"/>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="I8" s="46">
+        <f t="shared" si="1"/>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="J8" s="46">
+        <f t="shared" si="1"/>
+        <v>1.1263056648526228</v>
+      </c>
+      <c r="L8" s="8" t="str">
+        <f t="shared" ref="L8:L15" si="2">P8</f>
         <v>MKr10</v>
       </c>
-      <c r="H8" s="8" t="str">
-        <f>$K$7</f>
+      <c r="M8" s="8" t="str">
+        <f>$P$7</f>
         <v>MKr20</v>
       </c>
-      <c r="K8" s="60" t="s">
+      <c r="P8" s="60" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>101</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="46">
-        <f>1/M25</f>
+        <f>1/R25</f>
         <v>1.0988347949781687</v>
       </c>
-      <c r="G9" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F9" s="46">
+        <f t="shared" ref="F9:J18" si="3">E9</f>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="G9" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="H9" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="I9" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="J9" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0988347949781687</v>
+      </c>
+      <c r="L9" s="8" t="str">
+        <f t="shared" si="2"/>
         <v>MKr11</v>
       </c>
-      <c r="H9" s="8" t="str">
-        <f t="shared" ref="H9:H17" si="1">$K$7</f>
+      <c r="M9" s="8" t="str">
+        <f t="shared" ref="M9:M17" si="4">$P$7</f>
         <v>MKr20</v>
       </c>
-      <c r="K9" s="60" t="s">
+      <c r="P9" s="60" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>101</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="46">
-        <f>1/N25</f>
+        <f>1/S25</f>
         <v>1.074129809362824</v>
       </c>
-      <c r="G10" s="8" t="str">
-        <f>K10</f>
+      <c r="F10" s="46">
+        <f t="shared" si="3"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="G10" s="46">
+        <f t="shared" si="3"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="H10" s="46">
+        <f t="shared" si="3"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="I10" s="46">
+        <f t="shared" si="3"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="J10" s="46">
+        <f t="shared" si="3"/>
+        <v>1.074129809362824</v>
+      </c>
+      <c r="L10" s="8" t="str">
+        <f>P10</f>
         <v>MKr12</v>
       </c>
-      <c r="H10" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="M10" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>MKr20</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="P10" s="60" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>101</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="46">
-        <f>1/O25</f>
+        <f>1/T25</f>
         <v>1.0489548919558829</v>
       </c>
-      <c r="G11" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F11" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="G11" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="H11" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="I11" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="J11" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0489548919558829</v>
+      </c>
+      <c r="L11" s="8" t="str">
+        <f t="shared" si="2"/>
         <v>MKr13</v>
       </c>
-      <c r="H11" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="M11" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>MKr20</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="P11" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>101</v>
       </c>
       <c r="D12"/>
       <c r="E12" s="46">
-        <f>1/P25</f>
+        <f>1/U25</f>
         <v>1.0406298531308362</v>
       </c>
-      <c r="G12" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F12" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="G12" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="H12" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="I12" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="J12" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0406298531308362</v>
+      </c>
+      <c r="L12" s="8" t="str">
+        <f t="shared" si="2"/>
         <v>MKr14</v>
       </c>
-      <c r="H12" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="M12" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>MKr20</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="P12" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>101</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="46">
-        <f>1/Q25</f>
+        <f>1/V25</f>
         <v>1.0344233132513281</v>
       </c>
-      <c r="G13" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F13" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="G13" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="H13" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="I13" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="J13" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0344233132513281</v>
+      </c>
+      <c r="L13" s="8" t="str">
+        <f t="shared" si="2"/>
         <v>MKr15</v>
       </c>
-      <c r="H13" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="M13" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>MKr20</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="P13" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>101</v>
       </c>
       <c r="D14"/>
       <c r="E14" s="46">
-        <f>1/R25</f>
+        <f>1/W25</f>
         <v>1.0303021048320002</v>
       </c>
-      <c r="G14" s="8" t="str">
-        <f>K14</f>
+      <c r="F14" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="G14" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="H14" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="I14" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="J14" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0303021048320002</v>
+      </c>
+      <c r="L14" s="8" t="str">
+        <f>P14</f>
         <v>MKr16</v>
       </c>
-      <c r="H14" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="M14" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>MKr20</v>
       </c>
-      <c r="K14" s="60" t="s">
+      <c r="P14" s="60" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>101</v>
       </c>
       <c r="D15"/>
       <c r="E15" s="46">
-        <f>1/S25</f>
+        <f>1/X25</f>
         <v>1.0292728320000002</v>
       </c>
-      <c r="G15" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="F15" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="G15" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="H15" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="I15" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="J15" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0292728320000002</v>
+      </c>
+      <c r="L15" s="8" t="str">
+        <f t="shared" si="2"/>
         <v>MKr17</v>
       </c>
-      <c r="H15" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="M15" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>MKr20</v>
       </c>
-      <c r="K15" s="60" t="s">
+      <c r="P15" s="60" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>101</v>
       </c>
       <c r="D16"/>
       <c r="E16" s="46">
-        <f>1/T25</f>
+        <f>1/Y25</f>
         <v>1.0160640000000001</v>
       </c>
-      <c r="G16" s="8" t="str">
-        <f>K16</f>
+      <c r="F16" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="G16" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="H16" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="I16" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="J16" s="46">
+        <f t="shared" si="3"/>
+        <v>1.0160640000000001</v>
+      </c>
+      <c r="L16" s="8" t="str">
+        <f>P16</f>
         <v>MKr18</v>
       </c>
-      <c r="H16" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="M16" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>MKr20</v>
       </c>
-      <c r="K16" s="60" t="s">
+      <c r="P16" s="60" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="2:52" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:57" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>101</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="46">
-        <f>1/U25</f>
+        <f>1/Z25</f>
         <v>1.008</v>
       </c>
-      <c r="G17" s="8" t="str">
-        <f>K17</f>
+      <c r="F17" s="46">
+        <f t="shared" si="3"/>
+        <v>1.008</v>
+      </c>
+      <c r="G17" s="46">
+        <f t="shared" si="3"/>
+        <v>1.008</v>
+      </c>
+      <c r="H17" s="46">
+        <f t="shared" si="3"/>
+        <v>1.008</v>
+      </c>
+      <c r="I17" s="46">
+        <f t="shared" si="3"/>
+        <v>1.008</v>
+      </c>
+      <c r="J17" s="46">
+        <f t="shared" si="3"/>
+        <v>1.008</v>
+      </c>
+      <c r="L17" s="8" t="str">
+        <f>P17</f>
         <v>MKr19</v>
       </c>
-      <c r="H17" s="8" t="str">
-        <f t="shared" si="1"/>
+      <c r="M17" s="8" t="str">
+        <f t="shared" si="4"/>
         <v>MKr20</v>
       </c>
-      <c r="K17" s="60" t="s">
+      <c r="P17" s="60" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:57" ht="19.8" x14ac:dyDescent="0.4">
       <c r="B18" s="47"/>
       <c r="C18" s="47" t="s">
         <v>47</v>
@@ -3695,15 +3934,30 @@
       <c r="E18" s="49">
         <v>0.1</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="K18" s="29"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
+      <c r="F18" s="46">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="46">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="46">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="46">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="46">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="P18" s="29"/>
       <c r="Q18"/>
       <c r="R18"/>
       <c r="S18"/>
@@ -3740,8 +3994,13 @@
       <c r="AX18"/>
       <c r="AY18"/>
       <c r="AZ18"/>
-    </row>
-    <row r="19" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BD18"/>
+      <c r="BE18"/>
+    </row>
+    <row r="19" spans="2:57" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C19" s="10" t="s">
         <v>64</v>
       </c>
@@ -3752,15 +4011,25 @@
         <f>1-0.07</f>
         <v>0.92999999999999994</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="17">
+        <v>0.93</v>
+      </c>
+      <c r="G19" s="17">
+        <v>1</v>
+      </c>
+      <c r="H19" s="17">
+        <v>1</v>
+      </c>
+      <c r="I19" s="17">
+        <v>1</v>
+      </c>
+      <c r="J19" s="17">
+        <v>1</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="K19" s="29"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
+      <c r="P19" s="29"/>
       <c r="Q19"/>
       <c r="R19"/>
       <c r="S19"/>
@@ -3797,16 +4066,16 @@
       <c r="AX19"/>
       <c r="AY19"/>
       <c r="AZ19"/>
-    </row>
-    <row r="20" spans="2:52" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="K20" s="29" t="s">
+      <c r="BA19"/>
+      <c r="BB19"/>
+      <c r="BC19"/>
+      <c r="BD19"/>
+      <c r="BE19"/>
+    </row>
+    <row r="20" spans="2:57" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="P20" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
-      <c r="P20"/>
       <c r="Q20"/>
       <c r="R20"/>
       <c r="S20"/>
@@ -3843,19 +4112,19 @@
       <c r="AX20"/>
       <c r="AY20"/>
       <c r="AZ20"/>
-    </row>
-    <row r="21" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K21" s="55" t="s">
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+    </row>
+    <row r="21" spans="2:57" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P21" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="L21">
+      <c r="Q21">
         <v>2020</v>
       </c>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
       <c r="R21"/>
       <c r="S21"/>
       <c r="T21"/>
@@ -3891,36 +4160,36 @@
       <c r="AX21"/>
       <c r="AY21"/>
       <c r="AZ21"/>
-    </row>
-    <row r="22" spans="2:52" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K22" s="30" t="s">
+      <c r="BA21"/>
+      <c r="BB21"/>
+      <c r="BC21"/>
+      <c r="BD21"/>
+      <c r="BE21"/>
+    </row>
+    <row r="22" spans="2:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P22" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
       <c r="U22" s="31"/>
       <c r="V22" s="31"/>
       <c r="W22" s="31"/>
-      <c r="X22"/>
-      <c r="Y22"/>
-      <c r="Z22"/>
-      <c r="AA22"/>
-      <c r="AB22"/>
-      <c r="AC22" t="s">
-        <v>103</v>
-      </c>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31"/>
+      <c r="AC22"/>
       <c r="AD22"/>
       <c r="AE22"/>
       <c r="AF22"/>
       <c r="AG22"/>
-      <c r="AH22"/>
+      <c r="AH22" t="s">
+        <v>103</v>
+      </c>
       <c r="AI22"/>
       <c r="AJ22"/>
       <c r="AK22"/>
@@ -3939,530 +4208,520 @@
       <c r="AX22"/>
       <c r="AY22"/>
       <c r="AZ22"/>
-    </row>
-    <row r="23" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K23" s="32"/>
-      <c r="L23" s="33">
+      <c r="BA22"/>
+      <c r="BB22"/>
+      <c r="BC22"/>
+      <c r="BD22"/>
+      <c r="BE22"/>
+    </row>
+    <row r="23" spans="2:57" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P23" s="32"/>
+      <c r="Q23" s="33">
         <v>2010</v>
       </c>
-      <c r="M23" s="33">
+      <c r="R23" s="33">
         <v>2011</v>
       </c>
-      <c r="N23" s="33">
+      <c r="S23" s="33">
         <v>2012</v>
       </c>
-      <c r="O23" s="33">
+      <c r="T23" s="33">
         <v>2013</v>
       </c>
-      <c r="P23" s="33">
+      <c r="U23" s="33">
         <v>2014</v>
       </c>
-      <c r="Q23" s="33">
+      <c r="V23" s="33">
         <v>2015</v>
       </c>
-      <c r="R23" s="33">
+      <c r="W23" s="33">
         <v>2016</v>
       </c>
-      <c r="S23" s="33">
+      <c r="X23" s="33">
         <v>2017</v>
       </c>
-      <c r="T23" s="33">
+      <c r="Y23" s="33">
         <v>2018</v>
       </c>
-      <c r="U23" s="33">
+      <c r="Z23" s="33">
         <v>2019</v>
       </c>
-      <c r="V23" s="33">
+      <c r="AA23" s="33">
         <v>2020</v>
       </c>
-      <c r="W23" s="33">
+      <c r="AB23" s="33">
         <v>2021</v>
       </c>
-      <c r="X23" s="33">
+      <c r="AC23" s="33">
         <v>2022</v>
       </c>
-      <c r="Y23" s="33">
+      <c r="AD23" s="33">
         <v>2023</v>
       </c>
-      <c r="Z23" s="33">
+      <c r="AE23" s="33">
         <v>2024</v>
       </c>
-      <c r="AA23" s="33">
+      <c r="AF23" s="33">
         <v>2025</v>
       </c>
-      <c r="AB23" s="33">
+      <c r="AG23" s="33">
         <v>2026</v>
       </c>
-      <c r="AC23" s="33">
+      <c r="AH23" s="33">
         <v>2027</v>
       </c>
-      <c r="AD23" s="33">
+      <c r="AI23" s="33">
         <v>2028</v>
       </c>
-      <c r="AE23" s="33">
+      <c r="AJ23" s="33">
         <v>2029</v>
       </c>
-      <c r="AF23" s="33">
+      <c r="AK23" s="33">
         <v>2030</v>
       </c>
-      <c r="AG23" s="33">
+      <c r="AL23" s="33">
         <v>2031</v>
       </c>
-      <c r="AH23" s="33">
+      <c r="AM23" s="33">
         <v>2032</v>
       </c>
-      <c r="AI23" s="33">
+      <c r="AN23" s="33">
         <v>2033</v>
       </c>
-      <c r="AJ23" s="33">
+      <c r="AO23" s="33">
         <v>2034</v>
       </c>
-      <c r="AK23" s="33">
+      <c r="AP23" s="33">
         <v>2035</v>
       </c>
-      <c r="AL23" s="33">
+      <c r="AQ23" s="33">
         <v>2036</v>
       </c>
-      <c r="AM23" s="33">
+      <c r="AR23" s="33">
         <v>2037</v>
       </c>
-      <c r="AN23" s="33">
+      <c r="AS23" s="33">
         <v>2038</v>
       </c>
-      <c r="AO23" s="33">
+      <c r="AT23" s="33">
         <v>2039</v>
       </c>
-      <c r="AP23" s="33">
+      <c r="AU23" s="33">
         <v>2040</v>
       </c>
-      <c r="AQ23" s="33">
+      <c r="AV23" s="33">
         <v>2041</v>
       </c>
-      <c r="AR23" s="33">
+      <c r="AW23" s="33">
         <v>2042</v>
       </c>
-      <c r="AS23" s="33">
+      <c r="AX23" s="33">
         <v>2043</v>
       </c>
-      <c r="AT23" s="33">
+      <c r="AY23" s="33">
         <v>2044</v>
       </c>
-      <c r="AU23" s="33">
+      <c r="AZ23" s="33">
         <v>2045</v>
       </c>
-      <c r="AV23" s="33">
+      <c r="BA23" s="33">
         <v>2046</v>
       </c>
-      <c r="AW23" s="33">
+      <c r="BB23" s="33">
         <v>2047</v>
       </c>
-      <c r="AX23" s="33">
+      <c r="BC23" s="33">
         <v>2048</v>
       </c>
-      <c r="AY23" s="33">
+      <c r="BD23" s="33">
         <v>2049</v>
       </c>
-      <c r="AZ23" s="34">
+      <c r="BE23" s="34">
         <v>2050</v>
       </c>
     </row>
-    <row r="24" spans="2:52" x14ac:dyDescent="0.35">
-      <c r="K24" s="35" t="s">
+    <row r="24" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="P24" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="L24" s="36">
-        <v>1</v>
-      </c>
-      <c r="M24" s="36">
-        <f>L24*(L26)+L24</f>
+      <c r="Q24" s="36">
+        <v>1</v>
+      </c>
+      <c r="R24" s="36">
+        <f>Q24*(Q26)+Q24</f>
         <v>1.0249999999999999</v>
       </c>
-      <c r="N24" s="36">
-        <f t="shared" ref="N24:AZ24" si="2">M24*(M26)+M24</f>
+      <c r="S24" s="36">
+        <f t="shared" ref="S24:BE24" si="5">R24*(R26)+R24</f>
         <v>1.0485749999999998</v>
       </c>
-      <c r="O24" s="36">
-        <f t="shared" si="2"/>
+      <c r="T24" s="36">
+        <f t="shared" si="5"/>
         <v>1.0737407999999997</v>
       </c>
-      <c r="P24" s="36">
-        <f t="shared" si="2"/>
+      <c r="U24" s="36">
+        <f t="shared" si="5"/>
         <v>1.0823307263999997</v>
       </c>
-      <c r="Q24" s="36">
-        <f t="shared" si="2"/>
+      <c r="V24" s="36">
+        <f t="shared" si="5"/>
         <v>1.0888247107583997</v>
       </c>
-      <c r="R24" s="36">
-        <f t="shared" si="2"/>
+      <c r="W24" s="36">
+        <f t="shared" si="5"/>
         <v>1.0931800096014332</v>
       </c>
-      <c r="S24" s="36">
-        <f t="shared" si="2"/>
+      <c r="X24" s="36">
+        <f t="shared" si="5"/>
         <v>1.0942731896110347</v>
       </c>
-      <c r="T24" s="36">
-        <f t="shared" si="2"/>
+      <c r="Y24" s="36">
+        <f t="shared" si="5"/>
         <v>1.1084987410759781</v>
       </c>
-      <c r="U24" s="36">
-        <f t="shared" si="2"/>
+      <c r="Z24" s="36">
+        <f t="shared" si="5"/>
         <v>1.1173667310045861</v>
       </c>
-      <c r="V24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AA24" s="36">
+        <f t="shared" si="5"/>
         <v>1.1263056648526228</v>
       </c>
-      <c r="W24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AB24" s="36">
+        <f t="shared" si="5"/>
         <v>1.1296845818471808</v>
       </c>
-      <c r="X24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AC24" s="36">
+        <f t="shared" si="5"/>
         <v>1.143240796829347</v>
       </c>
-      <c r="Y24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AD24" s="36">
+        <f t="shared" si="5"/>
         <v>1.1603894087817872</v>
       </c>
-      <c r="Z24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AE24" s="36">
+        <f t="shared" si="5"/>
         <v>1.1801160287310777</v>
       </c>
-      <c r="AA24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AF24" s="36">
+        <f t="shared" si="5"/>
         <v>1.201358117248237</v>
       </c>
-      <c r="AB24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AG24" s="36">
+        <f t="shared" si="5"/>
         <v>1.2217812052414572</v>
       </c>
-      <c r="AC24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AH24" s="36">
+        <f t="shared" si="5"/>
         <v>1.2437732669358035</v>
       </c>
-      <c r="AD24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AI24" s="36">
+        <f t="shared" si="5"/>
         <v>1.2649174124737121</v>
       </c>
-      <c r="AE24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AJ24" s="36">
+        <f t="shared" si="5"/>
         <v>1.2876859258982389</v>
       </c>
-      <c r="AF24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AK24" s="36">
+        <f t="shared" si="5"/>
         <v>1.3108642725644073</v>
       </c>
-      <c r="AG24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AL24" s="36">
+        <f t="shared" si="5"/>
         <v>1.3331489651980022</v>
       </c>
-      <c r="AH24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AM24" s="36">
+        <f t="shared" si="5"/>
         <v>1.3584787955367643</v>
       </c>
-      <c r="AI24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AN24" s="36">
+        <f t="shared" si="5"/>
         <v>1.3829314138564262</v>
       </c>
-      <c r="AJ24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AO24" s="36">
+        <f t="shared" si="5"/>
         <v>1.4092071107196982</v>
       </c>
-      <c r="AK24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AP24" s="36">
+        <f t="shared" si="5"/>
         <v>1.4345728387126528</v>
       </c>
-      <c r="AL24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AQ24" s="36">
+        <f t="shared" si="5"/>
         <v>1.4603951498094805</v>
       </c>
-      <c r="AM24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AR24" s="36">
+        <f t="shared" si="5"/>
         <v>1.4896030528056701</v>
       </c>
-      <c r="AN24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AS24" s="36">
+        <f t="shared" si="5"/>
         <v>1.5179055108089778</v>
       </c>
-      <c r="AO24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AT24" s="36">
+        <f t="shared" si="5"/>
         <v>1.5467457155143485</v>
       </c>
-      <c r="AP24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AU24" s="36">
+        <f t="shared" si="5"/>
         <v>1.576133884109121</v>
       </c>
-      <c r="AQ24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AV24" s="36">
+        <f t="shared" si="5"/>
         <v>1.6060804279071943</v>
       </c>
-      <c r="AR24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AW24" s="36">
+        <f t="shared" si="5"/>
         <v>1.636595956037431</v>
       </c>
-      <c r="AS24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AX24" s="36">
+        <f t="shared" si="5"/>
         <v>1.6660546832461047</v>
       </c>
-      <c r="AT24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AY24" s="36">
+        <f t="shared" si="5"/>
         <v>1.6977097222277808</v>
       </c>
-      <c r="AU24" s="36">
-        <f t="shared" si="2"/>
+      <c r="AZ24" s="36">
+        <f t="shared" si="5"/>
         <v>1.7299662069501087</v>
       </c>
-      <c r="AV24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BA24" s="36">
+        <f t="shared" si="5"/>
         <v>1.7611055986752107</v>
       </c>
-      <c r="AW24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BB24" s="36">
+        <f t="shared" si="5"/>
         <v>1.7945666050500397</v>
       </c>
-      <c r="AX24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BC24" s="36">
+        <f t="shared" si="5"/>
         <v>1.8268688039409404</v>
       </c>
-      <c r="AY24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BD24" s="36">
+        <f t="shared" si="5"/>
         <v>1.8615793112158183</v>
       </c>
-      <c r="AZ24" s="36">
-        <f t="shared" si="2"/>
+      <c r="BE24" s="36">
+        <f t="shared" si="5"/>
         <v>1.896949318128919</v>
       </c>
     </row>
-    <row r="25" spans="2:52" x14ac:dyDescent="0.35">
-      <c r="K25" s="35" t="s">
+    <row r="25" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="P25" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="L25" s="36">
-        <f>L24/HLOOKUP($L$21,$L$23:$AZ$24,2,FALSE)</f>
+      <c r="Q25" s="36">
+        <f>Q24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
         <v>0.88785844838208294</v>
       </c>
-      <c r="M25" s="36">
-        <f t="shared" ref="M25:AZ25" si="3">M24/HLOOKUP($L$21,$L$23:$AZ$24,2,FALSE)</f>
+      <c r="R25" s="36">
+        <f t="shared" ref="R25:BE25" si="6">R24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
         <v>0.91005490959163493</v>
       </c>
-      <c r="N25" s="36">
-        <f t="shared" si="3"/>
+      <c r="S25" s="36">
+        <f t="shared" si="6"/>
         <v>0.93098617251224236</v>
       </c>
-      <c r="O25" s="36">
-        <f t="shared" si="3"/>
+      <c r="T25" s="36">
+        <f t="shared" si="6"/>
         <v>0.95332984065253612</v>
       </c>
-      <c r="P25" s="36">
-        <f t="shared" si="3"/>
+      <c r="U25" s="36">
+        <f t="shared" si="6"/>
         <v>0.96095647937775641</v>
       </c>
-      <c r="Q25" s="36">
-        <f t="shared" si="3"/>
+      <c r="V25" s="36">
+        <f t="shared" si="6"/>
         <v>0.96672221825402294</v>
       </c>
-      <c r="R25" s="36">
-        <f t="shared" si="3"/>
+      <c r="W25" s="36">
+        <f t="shared" si="6"/>
         <v>0.97058910712703905</v>
       </c>
-      <c r="S25" s="36">
-        <f t="shared" si="3"/>
+      <c r="X25" s="36">
+        <f t="shared" si="6"/>
         <v>0.97155969623416605</v>
       </c>
-      <c r="T25" s="36">
-        <f t="shared" si="3"/>
+      <c r="Y25" s="36">
+        <f t="shared" si="6"/>
         <v>0.98418997228521021</v>
       </c>
-      <c r="U25" s="36">
-        <f t="shared" si="3"/>
+      <c r="Z25" s="36">
+        <f t="shared" si="6"/>
         <v>0.99206349206349198</v>
       </c>
-      <c r="V25" s="36">
-        <f>V24/HLOOKUP($L$21,$L$23:$AZ$24,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="W25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AA25" s="36">
+        <f>AA24/HLOOKUP($Q$21,$Q$23:$BE$24,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AB25" s="36">
+        <f t="shared" si="6"/>
         <v>1.0030000000000001</v>
       </c>
-      <c r="X25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AC25" s="36">
+        <f t="shared" si="6"/>
         <v>1.015036</v>
       </c>
-      <c r="Y25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AD25" s="36">
+        <f t="shared" si="6"/>
         <v>1.0302615400000001</v>
       </c>
-      <c r="Z25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AE25" s="36">
+        <f t="shared" si="6"/>
         <v>1.0477759861800002</v>
       </c>
-      <c r="AA25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AF25" s="36">
+        <f t="shared" si="6"/>
         <v>1.0666359539312402</v>
       </c>
-      <c r="AB25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AG25" s="36">
+        <f t="shared" si="6"/>
         <v>1.0847687651480713</v>
       </c>
-      <c r="AC25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AH25" s="36">
+        <f t="shared" si="6"/>
         <v>1.1042946029207368</v>
       </c>
-      <c r="AD25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AI25" s="36">
+        <f t="shared" si="6"/>
         <v>1.1230676111703892</v>
       </c>
-      <c r="AE25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AJ25" s="36">
+        <f t="shared" si="6"/>
         <v>1.1432828281714562</v>
       </c>
-      <c r="AF25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AK25" s="36">
+        <f t="shared" si="6"/>
         <v>1.1638619190785424</v>
       </c>
-      <c r="AG25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AL25" s="36">
+        <f t="shared" si="6"/>
         <v>1.1836475717028776</v>
       </c>
-      <c r="AH25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AM25" s="36">
+        <f t="shared" si="6"/>
         <v>1.2061368755652324</v>
       </c>
-      <c r="AI25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AN25" s="36">
+        <f t="shared" si="6"/>
         <v>1.2278473393254066</v>
       </c>
-      <c r="AJ25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AO25" s="36">
+        <f t="shared" si="6"/>
         <v>1.2511764387725892</v>
       </c>
-      <c r="AK25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AP25" s="36">
+        <f t="shared" si="6"/>
         <v>1.2736976146704959</v>
       </c>
-      <c r="AL25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AQ25" s="36">
+        <f t="shared" si="6"/>
         <v>1.2966241717345648</v>
       </c>
-      <c r="AM25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AR25" s="36">
+        <f t="shared" si="6"/>
         <v>1.322556655169256</v>
       </c>
-      <c r="AN25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AS25" s="36">
+        <f t="shared" si="6"/>
         <v>1.3476852316174721</v>
       </c>
-      <c r="AO25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AT25" s="36">
+        <f t="shared" si="6"/>
         <v>1.373291251018204</v>
       </c>
-      <c r="AP25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AU25" s="36">
+        <f t="shared" si="6"/>
         <v>1.3993837847875499</v>
       </c>
-      <c r="AQ25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AV25" s="36">
+        <f t="shared" si="6"/>
         <v>1.4259720766985133</v>
       </c>
-      <c r="AR25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AW25" s="36">
+        <f t="shared" si="6"/>
         <v>1.4530655461557851</v>
       </c>
-      <c r="AS25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AX25" s="36">
+        <f t="shared" si="6"/>
         <v>1.479220725986589</v>
       </c>
-      <c r="AT25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AY25" s="36">
+        <f t="shared" si="6"/>
         <v>1.5073259197803344</v>
       </c>
-      <c r="AU25" s="36">
-        <f t="shared" si="3"/>
+      <c r="AZ25" s="36">
+        <f t="shared" si="6"/>
         <v>1.5359651122561608</v>
       </c>
-      <c r="AV25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BA25" s="36">
+        <f t="shared" si="6"/>
         <v>1.5636124842767718</v>
       </c>
-      <c r="AW25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BB25" s="36">
+        <f t="shared" si="6"/>
         <v>1.5933211214780305</v>
       </c>
-      <c r="AX25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BC25" s="36">
+        <f t="shared" si="6"/>
         <v>1.6220009016646351</v>
       </c>
-      <c r="AY25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BD25" s="36">
+        <f t="shared" si="6"/>
         <v>1.652818918796263</v>
       </c>
-      <c r="AZ25" s="36">
-        <f t="shared" si="3"/>
+      <c r="BE25" s="36">
+        <f t="shared" si="6"/>
         <v>1.6842224782533921</v>
       </c>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.35">
-      <c r="K26" s="61" t="s">
+    <row r="26" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="P26" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="L26" s="38">
+      <c r="Q26" s="38">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M26" s="38">
+      <c r="R26" s="38">
         <v>2.3E-2</v>
       </c>
-      <c r="N26" s="38">
+      <c r="S26" s="38">
         <v>2.4E-2</v>
-      </c>
-      <c r="O26" s="38">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="P26" s="38">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="Q26" s="38">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="R26" s="38">
-        <v>1E-3</v>
-      </c>
-      <c r="S26" s="38">
-        <v>1.3000000000000001E-2</v>
       </c>
       <c r="T26" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="U26" s="38">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="V26" s="38">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="W26" s="38">
+        <v>1E-3</v>
+      </c>
+      <c r="X26" s="38">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="Y26" s="38">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="V26" s="38">
+      <c r="Z26" s="38">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AA26" s="38">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="W26" s="38">
+      <c r="AB26" s="38">
         <v>1.2E-2</v>
       </c>
-      <c r="X26" s="38">
+      <c r="AC26" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y26" s="38">
+      <c r="AD26" s="38">
         <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="Z26" s="38">
-        <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AA26" s="38">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="AB26" s="38">
-        <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AC26" s="38">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="AD26" s="38">
-        <v>1.8000000000000002E-2</v>
       </c>
       <c r="AE26" s="38">
         <v>1.8000000000000002E-2</v>
@@ -4471,40 +4730,40 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="AG26" s="38">
-        <v>1.9E-2</v>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="AH26" s="38">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AI26" s="38">
         <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AI26" s="38">
-        <v>1.9E-2</v>
       </c>
       <c r="AJ26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="AK26" s="38">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AL26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AM26" s="38">
         <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="AL26" s="38">
-        <v>0.02</v>
-      </c>
-      <c r="AM26" s="38">
-        <v>1.9E-2</v>
       </c>
       <c r="AN26" s="38">
         <v>1.9E-2</v>
       </c>
       <c r="AO26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="AP26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="AQ26" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="AR26" s="38">
         <v>1.9E-2</v>
-      </c>
-      <c r="AP26" s="38">
-        <v>1.9E-2</v>
-      </c>
-      <c r="AQ26" s="38">
-        <v>1.9E-2</v>
-      </c>
-      <c r="AR26" s="38">
-        <v>1.8000000000000002E-2</v>
       </c>
       <c r="AS26" s="38">
         <v>1.9E-2</v>
@@ -4513,7 +4772,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="AU26" s="38">
-        <v>1.8000000000000002E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AV26" s="38">
         <v>1.9E-2</v>
@@ -4530,28 +4789,28 @@
       <c r="AZ26" s="38">
         <v>1.8000000000000002E-2</v>
       </c>
-    </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.35">
-      <c r="K27" s="37" t="s">
+      <c r="BA26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BB26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="BC26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BD26" s="38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BE26" s="38">
+        <v>1.8000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:57" x14ac:dyDescent="0.25">
+      <c r="P27" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="L27" s="39">
+      <c r="Q27" s="39">
         <v>7.4470000000000001</v>
-      </c>
-      <c r="M27" s="39">
-        <v>7.4539999999999997</v>
-      </c>
-      <c r="N27" s="39">
-        <v>7.4539999999999997</v>
-      </c>
-      <c r="O27" s="39">
-        <v>7.4539999999999997</v>
-      </c>
-      <c r="P27" s="40">
-        <v>7.4539999999999997</v>
-      </c>
-      <c r="Q27" s="39">
-        <v>7.4539999999999997</v>
       </c>
       <c r="R27" s="39">
         <v>7.4539999999999997</v>
@@ -4562,7 +4821,7 @@
       <c r="T27" s="39">
         <v>7.4539999999999997</v>
       </c>
-      <c r="U27" s="39">
+      <c r="U27" s="40">
         <v>7.4539999999999997</v>
       </c>
       <c r="V27" s="39">
@@ -4655,188 +4914,198 @@
       <c r="AY27" s="39">
         <v>7.4539999999999997</v>
       </c>
-      <c r="AZ27" s="41">
+      <c r="AZ27" s="39">
         <v>7.4539999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="2:52" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K28" s="42" t="s">
+      <c r="BA27" s="39">
+        <v>7.4539999999999997</v>
+      </c>
+      <c r="BB27" s="39">
+        <v>7.4539999999999997</v>
+      </c>
+      <c r="BC27" s="39">
+        <v>7.4539999999999997</v>
+      </c>
+      <c r="BD27" s="39">
+        <v>7.4539999999999997</v>
+      </c>
+      <c r="BE27" s="41">
+        <v>7.4539999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P28" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="L28" s="43" t="str">
-        <f>L35</f>
+      <c r="Q28" s="43" t="str">
+        <f>Q35</f>
         <v>MBS</v>
       </c>
-      <c r="M28" s="43" t="str">
-        <f t="shared" ref="M28:AZ28" si="4">M35</f>
+      <c r="R28" s="43" t="str">
+        <f t="shared" ref="R28:BE28" si="7">R35</f>
         <v>Opdateret med DK2025</v>
       </c>
-      <c r="N28" s="43">
-        <f t="shared" si="4"/>
+      <c r="S28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O28" s="43" t="str">
-        <f t="shared" si="4"/>
+      <c r="T28" s="43" t="str">
+        <f t="shared" si="7"/>
         <v>https://fm.dk/udgivelser/2020/august/dk2025-en-groen-retfaerdig-og-ansvarlig-genopretning-af-dansk-oekonomi/</v>
       </c>
-      <c r="P28" s="43">
-        <f t="shared" si="4"/>
+      <c r="U28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="43">
-        <f t="shared" si="4"/>
+      <c r="V28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="R28" s="43">
-        <f t="shared" si="4"/>
+      <c r="W28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S28" s="43">
-        <f t="shared" si="4"/>
+      <c r="X28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T28" s="43">
-        <f t="shared" si="4"/>
+      <c r="Y28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="U28" s="43">
-        <f t="shared" si="4"/>
+      <c r="Z28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AA28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AB28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AC28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AD28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Z28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AE28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AA28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AF28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AG28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AC28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AH28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AI28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AE28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AJ28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AF28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AK28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AL28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AM28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AI28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AN28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AJ28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AO28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AP28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AL28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AQ28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AM28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AR28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AN28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AS28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AO28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AT28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AP28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AU28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AQ28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AV28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AR28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AW28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AS28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AX28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AT28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AY28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AU28" s="43">
-        <f t="shared" si="4"/>
+      <c r="AZ28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AV28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BA28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AW28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BB28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AX28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BC28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AY28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BD28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AZ28" s="43">
-        <f t="shared" si="4"/>
+      <c r="BE28" s="43">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K29" s="44" t="s">
+    <row r="29" spans="2:57" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P29" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
@@ -4844,11 +5113,11 @@
       <c r="U29" s="7"/>
       <c r="V29" s="7"/>
       <c r="W29" s="7"/>
-      <c r="X29"/>
-      <c r="Y29"/>
-      <c r="Z29"/>
-      <c r="AA29"/>
-      <c r="AB29"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
       <c r="AC29"/>
       <c r="AD29"/>
       <c r="AE29"/>
@@ -4873,14 +5142,14 @@
       <c r="AX29"/>
       <c r="AY29"/>
       <c r="AZ29"/>
-    </row>
-    <row r="30" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K30" s="56"/>
-      <c r="L30"/>
-      <c r="M30"/>
-      <c r="N30"/>
-      <c r="O30"/>
-      <c r="P30"/>
+      <c r="BA29"/>
+      <c r="BB29"/>
+      <c r="BC29"/>
+      <c r="BD29"/>
+      <c r="BE29"/>
+    </row>
+    <row r="30" spans="2:57" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P30" s="56"/>
       <c r="Q30"/>
       <c r="R30"/>
       <c r="S30"/>
@@ -4917,16 +5186,16 @@
       <c r="AX30"/>
       <c r="AY30"/>
       <c r="AZ30"/>
-    </row>
-    <row r="31" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K31" s="57" t="s">
+      <c r="BA30"/>
+      <c r="BB30"/>
+      <c r="BC30"/>
+      <c r="BD30"/>
+      <c r="BE30"/>
+    </row>
+    <row r="31" spans="2:57" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P31" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
       <c r="Q31"/>
       <c r="R31"/>
       <c r="S31"/>
@@ -4963,22 +5232,22 @@
       <c r="AX31"/>
       <c r="AY31"/>
       <c r="AZ31"/>
-    </row>
-    <row r="32" spans="2:52" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K32" s="58">
+      <c r="BA31"/>
+      <c r="BB31"/>
+      <c r="BC31"/>
+      <c r="BD31"/>
+      <c r="BE31"/>
+    </row>
+    <row r="32" spans="2:57" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P32" s="58">
         <v>41767</v>
       </c>
-      <c r="L32" s="59" t="s">
+      <c r="Q32" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="M32" s="59" t="s">
+      <c r="R32" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
       <c r="S32"/>
       <c r="T32"/>
       <c r="U32"/>
@@ -5013,23 +5282,23 @@
       <c r="AX32"/>
       <c r="AY32"/>
       <c r="AZ32"/>
-    </row>
-    <row r="33" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K33" s="58">
+      <c r="BA32"/>
+      <c r="BB32"/>
+      <c r="BC32"/>
+      <c r="BD32"/>
+      <c r="BE32"/>
+    </row>
+    <row r="33" spans="16:96" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P33" s="58">
         <v>42102</v>
       </c>
-      <c r="L33" s="59" t="s">
+      <c r="Q33" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="M33" s="59" t="s">
+      <c r="R33" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="N33"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
+      <c r="S33"/>
       <c r="T33" s="45"/>
       <c r="U33" s="45"/>
       <c r="V33" s="45"/>
@@ -5062,38 +5331,38 @@
       <c r="AW33" s="45"/>
       <c r="AX33" s="45"/>
       <c r="AY33" s="45"/>
-      <c r="AZ33"/>
-    </row>
-    <row r="34" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K34" s="64">
+      <c r="AZ33" s="45"/>
+      <c r="BA33" s="45"/>
+      <c r="BB33" s="45"/>
+      <c r="BC33" s="45"/>
+      <c r="BD33" s="45"/>
+      <c r="BE33"/>
+    </row>
+    <row r="34" spans="16:96" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P34" s="64">
         <v>42702</v>
       </c>
-      <c r="L34" s="69" t="s">
+      <c r="Q34" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="M34" s="59" t="s">
+      <c r="R34" s="59" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="K35" s="73">
+    <row r="35" spans="16:96" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="P35" s="73">
         <v>44351</v>
       </c>
-      <c r="L35" s="74" t="s">
+      <c r="Q35" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="M35" s="74" t="s">
+      <c r="R35" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="N35" s="67"/>
-      <c r="O35" s="75" t="s">
+      <c r="S35" s="67"/>
+      <c r="T35" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="P35" s="67"/>
-      <c r="Q35" s="67"/>
-      <c r="R35" s="67"/>
-      <c r="S35" s="67"/>
-      <c r="T35" s="67"/>
       <c r="U35" s="67"/>
       <c r="V35" s="67"/>
       <c r="W35" s="67"/>
@@ -5125,12 +5394,12 @@
       <c r="AW35" s="67"/>
       <c r="AX35" s="67"/>
       <c r="AY35" s="67"/>
-      <c r="AZ35" s="68"/>
-      <c r="BA35" s="65"/>
-      <c r="BB35" s="65"/>
-      <c r="BC35" s="65"/>
-      <c r="BD35" s="65"/>
-      <c r="BE35" s="65"/>
+      <c r="AZ35" s="67"/>
+      <c r="BA35" s="67"/>
+      <c r="BB35" s="67"/>
+      <c r="BC35" s="67"/>
+      <c r="BD35" s="67"/>
+      <c r="BE35" s="68"/>
       <c r="BF35" s="65"/>
       <c r="BG35" s="65"/>
       <c r="BH35" s="65"/>
@@ -5164,14 +5433,14 @@
       <c r="CJ35" s="65"/>
       <c r="CK35" s="65"/>
       <c r="CL35" s="65"/>
-      <c r="CM35" s="66"/>
-    </row>
-    <row r="36" spans="11:91" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="L36" s="62"/>
-      <c r="M36" s="62"/>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
+      <c r="CM35" s="65"/>
+      <c r="CN35" s="65"/>
+      <c r="CO35" s="65"/>
+      <c r="CP35" s="65"/>
+      <c r="CQ35" s="65"/>
+      <c r="CR35" s="66"/>
+    </row>
+    <row r="36" spans="16:96" ht="14.4" x14ac:dyDescent="0.3">
       <c r="Q36" s="62"/>
       <c r="R36" s="62"/>
       <c r="S36" s="62"/>
@@ -5207,31 +5476,61 @@
       <c r="AW36" s="62"/>
       <c r="AX36" s="62"/>
       <c r="AY36" s="62"/>
-      <c r="AZ36" s="63"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="AZ36" s="62"/>
+      <c r="BA36" s="62"/>
+      <c r="BB36" s="62"/>
+      <c r="BC36" s="62"/>
+      <c r="BD36" s="62"/>
+      <c r="BE36" s="63"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C52" s="10"/>
       <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53"/>
       <c r="C53" s="10"/>
       <c r="E53" s="17"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E56" s="9"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E57" s="9"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58"/>
       <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="O35" r:id="rId1" xr:uid="{2A5C4B4A-D7D5-4EDE-B99F-9E5AC5DB0C93}"/>
+    <hyperlink ref="T35" r:id="rId1" xr:uid="{2A5C4B4A-D7D5-4EDE-B99F-9E5AC5DB0C93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5248,22 +5547,22 @@
       <selection activeCell="L48" sqref="K48:L49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.53125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L2" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="12:16" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="3" spans="12:16" ht="13.8" x14ac:dyDescent="0.25">
       <c r="L3" s="13" t="s">
         <v>34</v>
       </c>
@@ -5280,7 +5579,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L4" t="s">
         <v>52</v>
       </c>
@@ -5297,7 +5596,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L5" t="s">
         <v>53</v>
       </c>
@@ -5314,7 +5613,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L6" t="s">
         <v>54</v>
       </c>
@@ -5345,19 +5644,19 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="10" width="11.86328125" customWidth="1"/>
+    <col min="8" max="10" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -5365,7 +5664,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
@@ -5375,7 +5674,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
@@ -5384,12 +5683,12 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
@@ -5409,7 +5708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>62</v>
       </c>

</xml_diff>